<commit_message>
initial drag ui, some texts
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2967CF28-91BE-499F-B306-053E3BFD1C54}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0913748C-F3DE-4B01-B2FD-98F2685FB594}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Key</t>
   </si>
@@ -44,6 +44,66 @@
   </si>
   <si>
     <t>Knights of the Force Academy</t>
+  </si>
+  <si>
+    <t>options</t>
+  </si>
+  <si>
+    <t>OPTIONS</t>
+  </si>
+  <si>
+    <t>music</t>
+  </si>
+  <si>
+    <t>MUSIC</t>
+  </si>
+  <si>
+    <t>sound</t>
+  </si>
+  <si>
+    <t>SOUND</t>
+  </si>
+  <si>
+    <t>on</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>off</t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>CLOSE</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>confirmDesc</t>
+  </si>
+  <si>
+    <t>Are you sure?</t>
+  </si>
+  <si>
+    <t>RESTART</t>
+  </si>
+  <si>
+    <t>confirmTitleRestart</t>
   </si>
 </sst>
 </file>
@@ -393,7 +453,7 @@
   <dimension ref="A1:D143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,6 +500,86 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+    </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
     </row>

</xml_diff>

<commit_message>
more ui stuff: options, confirm, some tweaks
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0913748C-F3DE-4B01-B2FD-98F2685FB594}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84B33C0-52A6-484F-A71B-8DF6E7255801}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Key</t>
   </si>
@@ -97,13 +97,16 @@
     <t>confirmDesc</t>
   </si>
   <si>
-    <t>Are you sure?</t>
-  </si>
-  <si>
     <t>RESTART</t>
   </si>
   <si>
     <t>confirmTitleRestart</t>
+  </si>
+  <si>
+    <t>restart</t>
+  </si>
+  <si>
+    <t>Are you sure you want to restart the level?</t>
   </si>
 </sst>
 </file>
@@ -453,7 +456,7 @@
   <dimension ref="A1:D143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,15 +572,29 @@
         <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>27</v>
       </c>
-      <c r="B13" t="s">
-        <v>26</v>
+      <c r="B14" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
more act 1-1 stuff (victory anim., aesthetics)
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84B33C0-52A6-484F-A71B-8DF6E7255801}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AC38F8-0F69-4687-8947-987F6B405C15}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Key</t>
   </si>
@@ -107,6 +107,15 @@
   </si>
   <si>
     <t>Are you sure you want to restart the level?</t>
+  </si>
+  <si>
+    <t>victory</t>
+  </si>
+  <si>
+    <t>VICTORY</t>
+  </si>
+  <si>
+    <t>victory_act_1_1</t>
   </si>
 </sst>
 </file>
@@ -456,7 +465,7 @@
   <dimension ref="A1:D143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,6 +606,22 @@
         <v>25</v>
       </c>
     </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+    </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
     </row>

</xml_diff>

<commit_message>
first law lesson stuff
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AC38F8-0F69-4687-8947-987F6B405C15}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB94DBB9-84A2-44E5-9F73-208F017A6B74}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
   <si>
     <t>Key</t>
   </si>
@@ -116,6 +116,111 @@
   </si>
   <si>
     <t>victory_act_1_1</t>
+  </si>
+  <si>
+    <t>You have rescued the princess!</t>
+  </si>
+  <si>
+    <t>newton_first_law_title</t>
+  </si>
+  <si>
+    <t>Newton's First Law</t>
+  </si>
+  <si>
+    <t>newton_at_rest</t>
+  </si>
+  <si>
+    <t>At Rest</t>
+  </si>
+  <si>
+    <t>newton_in_motion</t>
+  </si>
+  <si>
+    <t>In Motion</t>
+  </si>
+  <si>
+    <t>newton_first_law_dlg_1</t>
+  </si>
+  <si>
+    <t>newton_first_law_desc</t>
+  </si>
+  <si>
+    <t>newton_first_law_dlg_2</t>
+  </si>
+  <si>
+    <t>newton_first_law_dlg_3</t>
+  </si>
+  <si>
+    <t>A net external force means the sum of all forces acting on the object.</t>
+  </si>
+  <si>
+    <t>It looks like the princess has been taken hostage by these nefarious goblins!</t>
+  </si>
+  <si>
+    <t>newton_first_law_dlg_4</t>
+  </si>
+  <si>
+    <t>newton_first_law_dlg_5</t>
+  </si>
+  <si>
+    <t>newton_first_law_dlg_6</t>
+  </si>
+  <si>
+    <t>As you can see, the force of gravity is pulling the object towards the Earth.</t>
+  </si>
+  <si>
+    <t>You must now use your forces to push the block towards the watchtower for a daring rescue!</t>
+  </si>
+  <si>
+    <t>velocityX</t>
+  </si>
+  <si>
+    <t>velocity(x)</t>
+  </si>
+  <si>
+    <t>velocityY</t>
+  </si>
+  <si>
+    <t>velocity(y)</t>
+  </si>
+  <si>
+    <t>newton_net_force_zero</t>
+  </si>
+  <si>
+    <t>Net Force (Sum of Forces) = 0 N</t>
+  </si>
+  <si>
+    <t>Now that the object is on the ground, there is a force pushing it outwards from the surface.</t>
+  </si>
+  <si>
+    <t>Newton's first law states that an object at rest will remain at rest, and an object in motion will maintain a constant velocity unless acted upon by a net external force.</t>
+  </si>
+  <si>
+    <t>newton_first_law_dlg_1_2</t>
+  </si>
+  <si>
+    <t>Let me drop a large object from the sky to demonstrate.</t>
+  </si>
+  <si>
+    <t>forceGravity</t>
+  </si>
+  <si>
+    <t>Force Gravity</t>
+  </si>
+  <si>
+    <t>forceNormal</t>
+  </si>
+  <si>
+    <t>Force Normal</t>
+  </si>
+  <si>
+    <t>Adding both the gravity and normal force will result in zero net force. Therefore the object is at rest.</t>
+  </si>
+  <si>
+    <t>This is the normal force perpendicular to the surface that prevents the object from penetrating.</t>
+  </si>
+  <si>
+    <t>newton_first_law_dlg_3_2</t>
   </si>
 </sst>
 </file>
@@ -462,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D143"/>
+  <dimension ref="A1:D151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,69 +724,190 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B55" s="2"/>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B57" s="2"/>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B59" s="2"/>
-    </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B61" s="2"/>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="4"/>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="4"/>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B87" s="4"/>
+      <c r="B65" s="2"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="2"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" s="2"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="2"/>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73" s="4"/>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" s="4"/>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B101" s="3"/>
-    </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B103" s="4"/>
-    </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B115" s="2"/>
-    </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B119" s="2"/>
-    </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B120" s="2"/>
-    </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B121" s="2"/>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B95" s="4"/>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B97" s="4"/>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B109" s="3"/>
+    </row>
+    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B111" s="4"/>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B123" s="2"/>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B124" s="2"/>
-    </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B125" s="2"/>
-    </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B126" s="2"/>
-    </row>
     <row r="127" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B127" s="2"/>
     </row>
@@ -691,14 +917,35 @@
     <row r="129" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B129" s="2"/>
     </row>
+    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B131" s="2"/>
+    </row>
+    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B132" s="2"/>
+    </row>
+    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B133" s="2"/>
+    </row>
+    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B134" s="2"/>
+    </row>
+    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B135" s="2"/>
+    </row>
+    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B136" s="2"/>
+    </row>
     <row r="137" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B137" s="4"/>
-    </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B138" s="4"/>
-    </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B143" s="2"/>
+      <c r="B137" s="2"/>
+    </row>
+    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B145" s="4"/>
+    </row>
+    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B146" s="4"/>
+    </row>
+    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B151" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
more of the lesson stuff for act 1-1
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB94DBB9-84A2-44E5-9F73-208F017A6B74}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05391AE-6703-4672-BF8A-AEC6393032F4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
   <si>
     <t>Key</t>
   </si>
@@ -151,9 +151,6 @@
     <t>newton_first_law_dlg_3</t>
   </si>
   <si>
-    <t>A net external force means the sum of all forces acting on the object.</t>
-  </si>
-  <si>
     <t>It looks like the princess has been taken hostage by these nefarious goblins!</t>
   </si>
   <si>
@@ -166,12 +163,6 @@
     <t>newton_first_law_dlg_6</t>
   </si>
   <si>
-    <t>As you can see, the force of gravity is pulling the object towards the Earth.</t>
-  </si>
-  <si>
-    <t>You must now use your forces to push the block towards the watchtower for a daring rescue!</t>
-  </si>
-  <si>
     <t>velocityX</t>
   </si>
   <si>
@@ -184,24 +175,12 @@
     <t>velocity(y)</t>
   </si>
   <si>
-    <t>newton_net_force_zero</t>
-  </si>
-  <si>
-    <t>Net Force (Sum of Forces) = 0 N</t>
-  </si>
-  <si>
-    <t>Now that the object is on the ground, there is a force pushing it outwards from the surface.</t>
-  </si>
-  <si>
     <t>Newton's first law states that an object at rest will remain at rest, and an object in motion will maintain a constant velocity unless acted upon by a net external force.</t>
   </si>
   <si>
     <t>newton_first_law_dlg_1_2</t>
   </si>
   <si>
-    <t>Let me drop a large object from the sky to demonstrate.</t>
-  </si>
-  <si>
     <t>forceGravity</t>
   </si>
   <si>
@@ -217,10 +196,79 @@
     <t>Adding both the gravity and normal force will result in zero net force. Therefore the object is at rest.</t>
   </si>
   <si>
-    <t>This is the normal force perpendicular to the surface that prevents the object from penetrating.</t>
-  </si>
-  <si>
     <t>newton_first_law_dlg_3_2</t>
+  </si>
+  <si>
+    <t>newton_balanced_force</t>
+  </si>
+  <si>
+    <t>Balanced force.</t>
+  </si>
+  <si>
+    <t>newton_zero_accel</t>
+  </si>
+  <si>
+    <t>Acceleration = 0 m/s²</t>
+  </si>
+  <si>
+    <t>forceZeroNetForce</t>
+  </si>
+  <si>
+    <t>0 Net Force</t>
+  </si>
+  <si>
+    <t>A net external force is the sum of all forces acting on the object. If the net external force is zero, then there is no acceleration.</t>
+  </si>
+  <si>
+    <t>I will now drop a large object from the sky to demonstrate.</t>
+  </si>
+  <si>
+    <t>The gravity force is pulling the object towards the Earth, which allows it to fall in the first place.</t>
+  </si>
+  <si>
+    <t>The normal force is pushing the object outwards from the surface.</t>
+  </si>
+  <si>
+    <t>There are two forces currently acting on this object: gravity and normal force.</t>
+  </si>
+  <si>
+    <t>Gather your forces for a daring rescue!</t>
+  </si>
+  <si>
+    <t>Excellent! Now that the first block is in place, notice how it took a couple of knights to be able to move the block?</t>
+  </si>
+  <si>
+    <t>newton_first_law_inertia_dlg_1</t>
+  </si>
+  <si>
+    <t>newton_first_law_inertia_dlg_2</t>
+  </si>
+  <si>
+    <t>This is because of inertia, which causes the block to have more frictional force against the push force of the knights.</t>
+  </si>
+  <si>
+    <t>newton_first_law_inertia_dlg_3</t>
+  </si>
+  <si>
+    <t>Inertia is the tendency of a physical object to resist a change in motion. A change in motion requires acceleration due to net force.</t>
+  </si>
+  <si>
+    <t>The mass of an object determines the object’s amount of inertia. The unit of measurement shown here is in kg (kilograms), which is 1000 grams per 1 kilogram.</t>
+  </si>
+  <si>
+    <t>newton_first_law_inertia_dlg_4</t>
+  </si>
+  <si>
+    <t>So, the more mass an object has, the more resistance (inertia) it will have from change of motion.</t>
+  </si>
+  <si>
+    <t>newton_first_law_inertia_dlg_5</t>
+  </si>
+  <si>
+    <t>newton_first_law_inertia_dlg_6</t>
+  </si>
+  <si>
+    <t>I will now drop another object from the sky. This time with less mass. Just one more block to rescue our damsel in distress!</t>
   </si>
 </sst>
 </file>
@@ -567,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D151"/>
+  <dimension ref="A1:D153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,18 +772,18 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -765,7 +813,7 @@
         <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -786,94 +834,155 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B25" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>45</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>64</v>
+        <v>42</v>
+      </c>
+      <c r="B31" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="B32" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>47</v>
-      </c>
-      <c r="B33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B63" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
@@ -888,41 +997,38 @@
       <c r="B71" s="2"/>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B73" s="4"/>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B89" s="4"/>
-    </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B95" s="4"/>
+      <c r="B73" s="2"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B75" s="4"/>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B91" s="4"/>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B97" s="4"/>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B109" s="3"/>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B99" s="4"/>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B111" s="4"/>
-    </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B123" s="2"/>
-    </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B127" s="2"/>
-    </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B128" s="2"/>
+      <c r="B111" s="3"/>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B113" s="4"/>
+    </row>
+    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B125" s="2"/>
     </row>
     <row r="129" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B129" s="2"/>
     </row>
+    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B130" s="2"/>
+    </row>
     <row r="131" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B131" s="2"/>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B132" s="2"/>
-    </row>
     <row r="133" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B133" s="2"/>
     </row>
@@ -938,14 +1044,20 @@
     <row r="137" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B137" s="2"/>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B145" s="4"/>
-    </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B146" s="4"/>
-    </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B151" s="2"/>
+    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B138" s="2"/>
+    </row>
+    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B139" s="2"/>
+    </row>
+    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B147" s="4"/>
+    </row>
+    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B148" s="4"/>
+    </row>
+    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B153" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
goblin sprites, some tweaks in act 1-1 lesson
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05391AE-6703-4672-BF8A-AEC6393032F4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3041C422-9858-4BA7-A76D-67F7F56E817A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
   <si>
     <t>Key</t>
   </si>
@@ -235,40 +235,46 @@
     <t>Gather your forces for a daring rescue!</t>
   </si>
   <si>
-    <t>Excellent! Now that the first block is in place, notice how it took a couple of knights to be able to move the block?</t>
-  </si>
-  <si>
     <t>newton_first_law_inertia_dlg_1</t>
   </si>
   <si>
     <t>newton_first_law_inertia_dlg_2</t>
   </si>
   <si>
-    <t>This is because of inertia, which causes the block to have more frictional force against the push force of the knights.</t>
-  </si>
-  <si>
     <t>newton_first_law_inertia_dlg_3</t>
   </si>
   <si>
-    <t>Inertia is the tendency of a physical object to resist a change in motion. A change in motion requires acceleration due to net force.</t>
-  </si>
-  <si>
-    <t>The mass of an object determines the object’s amount of inertia. The unit of measurement shown here is in kg (kilograms), which is 1000 grams per 1 kilogram.</t>
-  </si>
-  <si>
     <t>newton_first_law_inertia_dlg_4</t>
   </si>
   <si>
-    <t>So, the more mass an object has, the more resistance (inertia) it will have from change of motion.</t>
-  </si>
-  <si>
     <t>newton_first_law_inertia_dlg_5</t>
   </si>
   <si>
-    <t>newton_first_law_inertia_dlg_6</t>
-  </si>
-  <si>
     <t>I will now drop another object from the sky. This time with less mass. Just one more block to rescue our damsel in distress!</t>
+  </si>
+  <si>
+    <t>Inertia is the tendency of any physical object to resist any change in motion. A change in motion is acceleration due to net force acting on the object.</t>
+  </si>
+  <si>
+    <t>The mass of an object determines the object’s inertia. The unit of measurement shown here is in kg (kilograms), which is 1000 grams per 1 kilogram.</t>
+  </si>
+  <si>
+    <t>The block's mass gives it more weight, which allows its frictional force to go against the pushing force of the knights.</t>
+  </si>
+  <si>
+    <t>forceFriction</t>
+  </si>
+  <si>
+    <t>Force Friction</t>
+  </si>
+  <si>
+    <t>forcePush</t>
+  </si>
+  <si>
+    <t>Force Push</t>
+  </si>
+  <si>
+    <t>Excellent! Notice how it took a couple of knights to push the block?</t>
   </si>
 </sst>
 </file>
@@ -618,7 +624,7 @@
   <dimension ref="A1:D153"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,122 +872,130 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B30" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>44</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>57</v>
+        <v>42</v>
+      </c>
+      <c r="B33" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" t="s">
-        <v>70</v>
+        <v>44</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="B36" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="B37" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>75</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
+      </c>
+      <c r="B38" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B39" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>80</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="B40" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>81</v>
-      </c>
-      <c r="B41" t="s">
-        <v>82</v>
+        <v>74</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>75</v>
+      </c>
+      <c r="B42" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
act 1-2 treasure, victory trigger
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3041C422-9858-4BA7-A76D-67F7F56E817A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A458D30A-5240-4C1E-A8D5-E506958C7C6F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="95">
   <si>
     <t>Key</t>
   </si>
@@ -275,6 +275,36 @@
   </si>
   <si>
     <t>Excellent! Notice how it took a couple of knights to push the block?</t>
+  </si>
+  <si>
+    <t>newton_first_law_2_inertia_dlg_1</t>
+  </si>
+  <si>
+    <t>newton_first_law_2_inertia_dlg_2</t>
+  </si>
+  <si>
+    <t>The contraption before you allows us to measure an object's weight on the left by methodically adding objects with known weight on the right.</t>
+  </si>
+  <si>
+    <t>newton_first_law_2_inertia_dlg_3</t>
+  </si>
+  <si>
+    <t>In this scenario, we will learn more about inertia, and how it relates to an object's mass.</t>
+  </si>
+  <si>
+    <t>The gravitational acceleration of Earth is 9.8 meters per second square.</t>
+  </si>
+  <si>
+    <t>Force is mass times acceleration.</t>
+  </si>
+  <si>
+    <t>newton_first_law_2_inertia_dlg_4</t>
+  </si>
+  <si>
+    <t>newton_first_law_2_inertia_dlg_5</t>
+  </si>
+  <si>
+    <t>Weight is essentially the gravitational force exerted on an object based on its mass. Here are two important things to know:</t>
   </si>
 </sst>
 </file>
@@ -623,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,6 +1028,46 @@
         <v>76</v>
       </c>
     </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>92</v>
+      </c>
+      <c r="B46" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>93</v>
+      </c>
+      <c r="B47" t="s">
+        <v>90</v>
+      </c>
+    </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
     </row>

</xml_diff>

<commit_message>
act 1-2 lessons stuff, victory modal
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A458D30A-5240-4C1E-A8D5-E506958C7C6F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C356EF50-F897-4A4F-A02E-A9843D6D00DA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="97">
   <si>
     <t>Key</t>
   </si>
@@ -277,34 +277,40 @@
     <t>Excellent! Notice how it took a couple of knights to push the block?</t>
   </si>
   <si>
-    <t>newton_first_law_2_inertia_dlg_1</t>
-  </si>
-  <si>
-    <t>newton_first_law_2_inertia_dlg_2</t>
-  </si>
-  <si>
-    <t>The contraption before you allows us to measure an object's weight on the left by methodically adding objects with known weight on the right.</t>
-  </si>
-  <si>
-    <t>newton_first_law_2_inertia_dlg_3</t>
-  </si>
-  <si>
-    <t>In this scenario, we will learn more about inertia, and how it relates to an object's mass.</t>
-  </si>
-  <si>
-    <t>The gravitational acceleration of Earth is 9.8 meters per second square.</t>
-  </si>
-  <si>
-    <t>Force is mass times acceleration.</t>
-  </si>
-  <si>
-    <t>newton_first_law_2_inertia_dlg_4</t>
-  </si>
-  <si>
-    <t>newton_first_law_2_inertia_dlg_5</t>
-  </si>
-  <si>
-    <t>Weight is essentially the gravitational force exerted on an object based on its mass. Here are two important things to know:</t>
+    <t>newton_first_law_inertia_2_dlg_1</t>
+  </si>
+  <si>
+    <t>newton_first_law_inertia_2_dlg_2</t>
+  </si>
+  <si>
+    <t>newton_first_law_inertia_2_dlg_3</t>
+  </si>
+  <si>
+    <t>newton_first_law_inertia_2_dlg_4</t>
+  </si>
+  <si>
+    <t>In this scenario, we will learn more about inertia, and how it relates to mass.</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Here's a locked treasure chest found in the dark recesses of a dungeon. Drag the correct amount of weights on the right platform to unlock it.</t>
+  </si>
+  <si>
+    <t>Observe how the forces interact on this balance scale.</t>
+  </si>
+  <si>
+    <t>The weight of the objects on each platform influences the tipping of the scale. If objects on both platforms have an equal amount of weight, they will align horizontally.</t>
+  </si>
+  <si>
+    <t>newton_first_law_inertia_2_victory</t>
+  </si>
+  <si>
+    <t>You have opened the treasure chest! Behold, the riches uncovered:</t>
   </si>
 </sst>
 </file>
@@ -651,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D153"/>
+  <dimension ref="A1:D154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -926,186 +932,194 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>41</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>42</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>58</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>45</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>46</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>71</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>72</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>73</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>74</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>75</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>85</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>86</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="B46" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>88</v>
       </c>
-      <c r="B45" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="B47" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B46" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>93</v>
-      </c>
-      <c r="B47" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="2"/>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" s="2"/>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" s="2"/>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="2"/>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B73" s="2"/>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="4"/>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B91" s="4"/>
-    </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B97" s="4"/>
-    </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B99" s="4"/>
-    </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B111" s="3"/>
-    </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B113" s="4"/>
-    </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B125" s="2"/>
-    </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B129" s="2"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>95</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="2"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" s="2"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" s="2"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" s="2"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B74" s="2"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B76" s="4"/>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B92" s="4"/>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B98" s="4"/>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B100" s="4"/>
+    </row>
+    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B112" s="3"/>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B114" s="4"/>
+    </row>
+    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B126" s="2"/>
     </row>
     <row r="130" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B130" s="2"/>
@@ -1113,8 +1127,8 @@
     <row r="131" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B131" s="2"/>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B133" s="2"/>
+    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B132" s="2"/>
     </row>
     <row r="134" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B134" s="2"/>
@@ -1134,14 +1148,17 @@
     <row r="139" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B139" s="2"/>
     </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B147" s="4"/>
+    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B140" s="2"/>
     </row>
     <row r="148" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B148" s="4"/>
     </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B153" s="2"/>
+    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B149" s="4"/>
+    </row>
+    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B154" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
initial geometry art assets for act 2
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C356EF50-F897-4A4F-A02E-A9843D6D00DA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C975CE6-254C-4B08-9C42-CCF3C23A5983}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="99">
   <si>
     <t>Key</t>
   </si>
@@ -311,6 +311,12 @@
   </si>
   <si>
     <t>You have opened the treasure chest! Behold, the riches uncovered:</t>
+  </si>
+  <si>
+    <t>launch</t>
+  </si>
+  <si>
+    <t>LAUNCH</t>
   </si>
 </sst>
 </file>
@@ -657,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D154"/>
+  <dimension ref="A1:D155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,189 +946,194 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="B31" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>52</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>41</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>42</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>58</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>44</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B37" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>45</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>46</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>71</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>72</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>73</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>74</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>75</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>85</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B45" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>86</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>87</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>88</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B48" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>95</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B49" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C48">
+      <c r="C49">
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="2"/>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" s="2"/>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="2"/>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72" s="2"/>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B74" s="2"/>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76" s="4"/>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B92" s="4"/>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B98" s="4"/>
-    </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B100" s="4"/>
-    </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B112" s="3"/>
-    </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B114" s="4"/>
-    </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B126" s="2"/>
-    </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B130" s="2"/>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="2"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" s="2"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="2"/>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73" s="2"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B75" s="2"/>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B77" s="4"/>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B93" s="4"/>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B99" s="4"/>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B101" s="4"/>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B113" s="3"/>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B115" s="4"/>
+    </row>
+    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B127" s="2"/>
     </row>
     <row r="131" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B131" s="2"/>
@@ -1130,8 +1141,8 @@
     <row r="132" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B132" s="2"/>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B134" s="2"/>
+    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B133" s="2"/>
     </row>
     <row r="135" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B135" s="2"/>
@@ -1151,14 +1162,17 @@
     <row r="140" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B140" s="2"/>
     </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B148" s="4"/>
+    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B141" s="2"/>
     </row>
     <row r="149" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B149" s="4"/>
     </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B154" s="2"/>
+    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B150" s="4"/>
+    </row>
+    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B155" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added y-graph, toggle graph, prep dialogs in act 2-1
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0B9E06-525D-4A73-B25A-E1DD83F6FAE2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877730F0-A130-491B-9D0C-B9CA0FEADC34}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="112">
   <si>
     <t>Key</t>
   </si>
@@ -341,6 +341,21 @@
   </si>
   <si>
     <t>Time (seconds)</t>
+  </si>
+  <si>
+    <t>axis</t>
+  </si>
+  <si>
+    <t>Axis</t>
+  </si>
+  <si>
+    <t>newton_second_law_title</t>
+  </si>
+  <si>
+    <t>newton_second_law_desc</t>
+  </si>
+  <si>
+    <t>Newton's Second Law</t>
   </si>
 </sst>
 </file>
@@ -687,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D159"/>
+  <dimension ref="A1:D160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,205 +1009,229 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B34" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B35" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="B36" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B38" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B39" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="B40" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>44</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="B41" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>45</v>
-      </c>
-      <c r="B42" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B45" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B46" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>74</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
+      </c>
+      <c r="B47" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>75</v>
-      </c>
-      <c r="B48" t="s">
-        <v>76</v>
+        <v>74</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>85</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>89</v>
+        <v>75</v>
+      </c>
+      <c r="B49" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>86</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>93</v>
+        <v>85</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>87</v>
-      </c>
-      <c r="B51" t="s">
-        <v>94</v>
+        <v>86</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>88</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
+      </c>
+      <c r="B52" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>95</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B54" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C53">
+      <c r="C54">
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="2"/>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B73" s="2"/>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="2"/>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B77" s="2"/>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B79" s="2"/>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="4"/>
-    </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B97" s="4"/>
-    </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B103" s="4"/>
-    </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B105" s="4"/>
-    </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B117" s="3"/>
-    </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B119" s="4"/>
-    </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B131" s="2"/>
-    </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B135" s="2"/>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>109</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" s="2"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B74" s="2"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B76" s="2"/>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B78" s="2"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B80" s="2"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" s="4"/>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B98" s="4"/>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B104" s="4"/>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B106" s="4"/>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B118" s="3"/>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B120" s="4"/>
+    </row>
+    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B132" s="2"/>
     </row>
     <row r="136" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B136" s="2"/>
@@ -1200,8 +1239,8 @@
     <row r="137" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B137" s="2"/>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B139" s="2"/>
+    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B138" s="2"/>
     </row>
     <row r="140" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B140" s="2"/>
@@ -1221,14 +1260,17 @@
     <row r="145" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B145" s="2"/>
     </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B153" s="4"/>
+    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B146" s="2"/>
     </row>
     <row r="154" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B154" s="4"/>
     </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B159" s="2"/>
+    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B155" s="4"/>
+    </row>
+    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B160" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
act 2-1 explanation and such
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877730F0-A130-491B-9D0C-B9CA0FEADC34}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49403910-33F3-49A6-9F93-695A13C458A7}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="163">
   <si>
     <t>Key</t>
   </si>
@@ -356,6 +356,159 @@
   </si>
   <si>
     <t>Newton's Second Law</t>
+  </si>
+  <si>
+    <t>forceBalanced</t>
+  </si>
+  <si>
+    <t>force</t>
+  </si>
+  <si>
+    <t>Force</t>
+  </si>
+  <si>
+    <t>Force Balanced</t>
+  </si>
+  <si>
+    <t>forceUnbalanced</t>
+  </si>
+  <si>
+    <t>Force Unbalanced</t>
+  </si>
+  <si>
+    <t>knightPushing</t>
+  </si>
+  <si>
+    <t>Knight Pushing</t>
+  </si>
+  <si>
+    <t>constantMotion</t>
+  </si>
+  <si>
+    <t>Constant Motion</t>
+  </si>
+  <si>
+    <t>falling</t>
+  </si>
+  <si>
+    <t>pressLaunch</t>
+  </si>
+  <si>
+    <t>pressGraph</t>
+  </si>
+  <si>
+    <t>Press the GRAPH button.</t>
+  </si>
+  <si>
+    <t>Press the LAUNCH button.</t>
+  </si>
+  <si>
+    <t>Falling due to Gravity</t>
+  </si>
+  <si>
+    <t>mass</t>
+  </si>
+  <si>
+    <t>Mass</t>
+  </si>
+  <si>
+    <t>accel</t>
+  </si>
+  <si>
+    <t>Acceleration</t>
+  </si>
+  <si>
+    <t>vector</t>
+  </si>
+  <si>
+    <t>Vector</t>
+  </si>
+  <si>
+    <t>vel</t>
+  </si>
+  <si>
+    <t>Velocity</t>
+  </si>
+  <si>
+    <t>direction</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>magnitude</t>
+  </si>
+  <si>
+    <t>Magnitude</t>
+  </si>
+  <si>
+    <t>Newton’s second law states that the acceleration of an object equals the net force acting on the object over the object’s mass.</t>
+  </si>
+  <si>
+    <t>newton_second_law_dlg_1</t>
+  </si>
+  <si>
+    <t>Acceleration is what causes an object’s velocity to change over time. Which means the object will speed up, slow down, or change direction.</t>
+  </si>
+  <si>
+    <t>newton_second_law_dlg_2</t>
+  </si>
+  <si>
+    <t>Here are the equations for both the net force (F-net), and acceleration (A). Where mass is kilograms (kg), distance is meters (m), and time is seconds (s).</t>
+  </si>
+  <si>
+    <t>newton_second_law_dlg_3</t>
+  </si>
+  <si>
+    <t>As you can see, the more the mass the object have, the less it will accelerate from the net force.</t>
+  </si>
+  <si>
+    <t>newton_second_law_dlg_4</t>
+  </si>
+  <si>
+    <t>Note that: force, acceleration, and velocity are all vectors.  This means that they all have a direction, and a magnitude.</t>
+  </si>
+  <si>
+    <t>newton_second_law_dlg_5</t>
+  </si>
+  <si>
+    <t>Now let’s see this in action!</t>
+  </si>
+  <si>
+    <t>newton_second_law_dlg_6</t>
+  </si>
+  <si>
+    <t>A brave sir knight has brought us a wheel to demonstrate. The wheel is enchanted with magical trails to allow us to observe its motion.</t>
+  </si>
+  <si>
+    <t>newton_second_law_dlg_7</t>
+  </si>
+  <si>
+    <t>Observe how each trail’s distance starts to increase around this area. This shows us the force being applied to the wheel.</t>
+  </si>
+  <si>
+    <t>Now around this area, the distance between each trail is the same. This tells us that the net force on the wheel equals zero.</t>
+  </si>
+  <si>
+    <t>newton_second_law_dlg_8</t>
+  </si>
+  <si>
+    <t>newton_second_law_dlg_9</t>
+  </si>
+  <si>
+    <t>Here we can see the trails go down. From here we can observe that the only force acting on the wheel is the gravity.</t>
+  </si>
+  <si>
+    <t>The nefarious goblins have appeared out of thin air! They are surely up to no good. Get rid of them by using the wheel!</t>
+  </si>
+  <si>
+    <t>newton_second_law_dlg_10</t>
+  </si>
+  <si>
+    <t>examples</t>
+  </si>
+  <si>
+    <t>Examples</t>
   </si>
 </sst>
 </file>
@@ -702,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D160"/>
+  <dimension ref="A1:D168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,283 +1130,459 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>90</v>
+        <v>113</v>
       </c>
       <c r="B30" t="s">
-        <v>91</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="B31" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B32" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B33" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B34" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B35" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B36" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>107</v>
       </c>
       <c r="B37" t="s">
-        <v>65</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>52</v>
+        <v>105</v>
       </c>
       <c r="B38" t="s">
-        <v>66</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="B39" t="s">
-        <v>69</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>44</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>57</v>
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="B44" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>71</v>
-      </c>
-      <c r="B45" t="s">
-        <v>84</v>
+        <v>44</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>74</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
+      </c>
+      <c r="B48" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B49" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>85</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>89</v>
+        <v>73</v>
+      </c>
+      <c r="B50" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B52" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>88</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>92</v>
+        <v>85</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>95</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C54">
-        <v>4</v>
+        <v>86</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>109</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C55">
-        <v>2</v>
+        <v>87</v>
+      </c>
+      <c r="B55" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>88</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>95</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C57">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>118</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>120</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>122</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>109</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>110</v>
       </c>
-      <c r="B56" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72" s="2"/>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B74" s="2"/>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76" s="2"/>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B78" s="2"/>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B80" s="2"/>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" s="4"/>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B98" s="4"/>
-    </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B104" s="4"/>
+      <c r="B62" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>123</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>124</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>128</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>130</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>134</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>132</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>136</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>138</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>161</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>141</v>
+      </c>
+      <c r="B72" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>143</v>
+      </c>
+      <c r="B73" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>145</v>
+      </c>
+      <c r="B74" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>147</v>
+      </c>
+      <c r="B75" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>149</v>
+      </c>
+      <c r="B76" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>151</v>
+      </c>
+      <c r="B77" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>153</v>
+      </c>
+      <c r="B78" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>156</v>
+      </c>
+      <c r="B79" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>157</v>
+      </c>
+      <c r="B80" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>160</v>
+      </c>
+      <c r="B81" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B82" s="2"/>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B84" s="2"/>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B86" s="2"/>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B88" s="2"/>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B90" s="4"/>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B106" s="4"/>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B118" s="3"/>
-    </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B120" s="4"/>
-    </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B132" s="2"/>
-    </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B136" s="2"/>
-    </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B137" s="2"/>
-    </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B138" s="2"/>
+    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B112" s="4"/>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B114" s="4"/>
+    </row>
+    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B126" s="3"/>
+    </row>
+    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B128" s="4"/>
     </row>
     <row r="140" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B140" s="2"/>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B141" s="2"/>
-    </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B142" s="2"/>
-    </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B143" s="2"/>
-    </row>
     <row r="144" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B144" s="2"/>
     </row>
@@ -1263,14 +1592,35 @@
     <row r="146" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B146" s="2"/>
     </row>
+    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B148" s="2"/>
+    </row>
+    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B149" s="2"/>
+    </row>
+    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B150" s="2"/>
+    </row>
+    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B151" s="2"/>
+    </row>
+    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B152" s="2"/>
+    </row>
+    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B153" s="2"/>
+    </row>
     <row r="154" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B154" s="4"/>
-    </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B155" s="4"/>
-    </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B160" s="2"/>
+      <c r="B154" s="2"/>
+    </row>
+    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B162" s="4"/>
+    </row>
+    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B163" s="4"/>
+    </row>
+    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B168" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
act 2-1 explanations implemented
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49403910-33F3-49A6-9F93-695A13C458A7}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1940DABF-1EEF-42E1-BE65-10F76EF7D842}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="165">
   <si>
     <t>Key</t>
   </si>
@@ -460,21 +460,12 @@
     <t>newton_second_law_dlg_3</t>
   </si>
   <si>
-    <t>As you can see, the more the mass the object have, the less it will accelerate from the net force.</t>
-  </si>
-  <si>
     <t>newton_second_law_dlg_4</t>
   </si>
   <si>
-    <t>Note that: force, acceleration, and velocity are all vectors.  This means that they all have a direction, and a magnitude.</t>
-  </si>
-  <si>
     <t>newton_second_law_dlg_5</t>
   </si>
   <si>
-    <t>Now let’s see this in action!</t>
-  </si>
-  <si>
     <t>newton_second_law_dlg_6</t>
   </si>
   <si>
@@ -487,28 +478,43 @@
     <t>Observe how each trail’s distance starts to increase around this area. This shows us the force being applied to the wheel.</t>
   </si>
   <si>
-    <t>Now around this area, the distance between each trail is the same. This tells us that the net force on the wheel equals zero.</t>
-  </si>
-  <si>
     <t>newton_second_law_dlg_8</t>
   </si>
   <si>
     <t>newton_second_law_dlg_9</t>
   </si>
   <si>
-    <t>Here we can see the trails go down. From here we can observe that the only force acting on the wheel is the gravity.</t>
-  </si>
-  <si>
     <t>The nefarious goblins have appeared out of thin air! They are surely up to no good. Get rid of them by using the wheel!</t>
   </si>
   <si>
-    <t>newton_second_law_dlg_10</t>
-  </si>
-  <si>
     <t>examples</t>
   </si>
   <si>
     <t>Examples</t>
+  </si>
+  <si>
+    <t>newton_second_law_dlg_4_2</t>
+  </si>
+  <si>
+    <t>Note that: force, acceleration, and velocity are all vectors.</t>
+  </si>
+  <si>
+    <t>As you can see, the more mass an object has, the less it will accelerate from the net force.</t>
+  </si>
+  <si>
+    <t>At this point the trails are going down. We can observe that the only force acting on the wheel is the gravity.</t>
+  </si>
+  <si>
+    <t>Around here, the distance between each trail is the same. This tells us that the net force on the wheel equals zero.</t>
+  </si>
+  <si>
+    <t>A vector is composed of a value for each axis. In our case, the x and y. These values can also tell us the direction, and the magnitude (for example: speed).</t>
+  </si>
+  <si>
+    <t>dragForceSlider</t>
+  </si>
+  <si>
+    <t>Drag the slider to change the Force value.</t>
   </si>
 </sst>
 </file>
@@ -855,10 +861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D168"/>
+  <dimension ref="A1:D169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1416,175 +1422,180 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>128</v>
+        <v>163</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>129</v>
+        <v>164</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>161</v>
+        <v>138</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>141</v>
-      </c>
-      <c r="B72" t="s">
-        <v>142</v>
+        <v>155</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B73" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B74" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B75" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B76" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="B77" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B78" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B79" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B80" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>152</v>
+      </c>
+      <c r="B81" t="s">
         <v>160</v>
       </c>
-      <c r="B81" t="s">
-        <v>159</v>
-      </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B82" s="2"/>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B84" s="2"/>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B86" s="2"/>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B88" s="2"/>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B90" s="4"/>
-    </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B106" s="4"/>
-    </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B112" s="4"/>
-    </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B114" s="4"/>
-    </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B126" s="3"/>
-    </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B128" s="4"/>
-    </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B140" s="2"/>
-    </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B144" s="2"/>
+      <c r="A82" t="s">
+        <v>153</v>
+      </c>
+      <c r="B82" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B83" s="2"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B85" s="2"/>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B87" s="2"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B89" s="2"/>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B91" s="4"/>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B107" s="4"/>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B113" s="4"/>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B115" s="4"/>
+    </row>
+    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B127" s="3"/>
+    </row>
+    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B129" s="4"/>
+    </row>
+    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B141" s="2"/>
     </row>
     <row r="145" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B145" s="2"/>
@@ -1592,8 +1603,8 @@
     <row r="146" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B146" s="2"/>
     </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B148" s="2"/>
+    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B147" s="2"/>
     </row>
     <row r="149" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B149" s="2"/>
@@ -1613,14 +1624,17 @@
     <row r="154" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B154" s="2"/>
     </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B162" s="4"/>
+    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B155" s="2"/>
     </row>
     <row r="163" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B163" s="4"/>
     </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B168" s="2"/>
+    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B164" s="4"/>
+    </row>
+    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B169" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
some tweaks to act 2-1, wrap up act 2-1
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1940DABF-1EEF-42E1-BE65-10F76EF7D842}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11444EA8-FBCB-4F37-AF9B-3A774CB535F9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="175">
   <si>
     <t>Key</t>
   </si>
@@ -340,9 +340,6 @@
     <t>timeSlider</t>
   </si>
   <si>
-    <t>Time (seconds)</t>
-  </si>
-  <si>
     <t>axis</t>
   </si>
   <si>
@@ -469,15 +466,9 @@
     <t>newton_second_law_dlg_6</t>
   </si>
   <si>
-    <t>A brave sir knight has brought us a wheel to demonstrate. The wheel is enchanted with magical trails to allow us to observe its motion.</t>
-  </si>
-  <si>
     <t>newton_second_law_dlg_7</t>
   </si>
   <si>
-    <t>Observe how each trail’s distance starts to increase around this area. This shows us the force being applied to the wheel.</t>
-  </si>
-  <si>
     <t>newton_second_law_dlg_8</t>
   </si>
   <si>
@@ -502,19 +493,58 @@
     <t>As you can see, the more mass an object has, the less it will accelerate from the net force.</t>
   </si>
   <si>
-    <t>At this point the trails are going down. We can observe that the only force acting on the wheel is the gravity.</t>
-  </si>
-  <si>
-    <t>Around here, the distance between each trail is the same. This tells us that the net force on the wheel equals zero.</t>
-  </si>
-  <si>
-    <t>A vector is composed of a value for each axis. In our case, the x and y. These values can also tell us the direction, and the magnitude (for example: speed).</t>
-  </si>
-  <si>
     <t>dragForceSlider</t>
   </si>
   <si>
     <t>Drag the slider to change the Force value.</t>
+  </si>
+  <si>
+    <t>Time: {0:0.0} - {1:0.0} seconds</t>
+  </si>
+  <si>
+    <t>newton_second_law_graph_1</t>
+  </si>
+  <si>
+    <t>The graph maps out the trails across time along the x and y axis. Be sure to check the velocity and acceleration by scrolling down.</t>
+  </si>
+  <si>
+    <t>newton_second_law_graph_2</t>
+  </si>
+  <si>
+    <t>newton_second_law_graph_3</t>
+  </si>
+  <si>
+    <t>Observe how the position line curves as velocity increases, indicating that there is acceleration.</t>
+  </si>
+  <si>
+    <t>If the position line is straight, then velocity is constant, and therefore no acceleration.</t>
+  </si>
+  <si>
+    <t>pressToProceed</t>
+  </si>
+  <si>
+    <t>targetsEliminated</t>
+  </si>
+  <si>
+    <t>Targets Eliminated</t>
+  </si>
+  <si>
+    <t>Press this button once you are finish.</t>
+  </si>
+  <si>
+    <t>At this point, the distance between each trail is equal. This means that the net force acting on the wheel equals zero.</t>
+  </si>
+  <si>
+    <t>The trails here are going down. We can observe that the only force acting on the wheel is the gravity.</t>
+  </si>
+  <si>
+    <t>A valiant knight has brought us a wheel to demonstrate. The wheel is enchanted with magical trails to allow us to observe its motion.</t>
+  </si>
+  <si>
+    <t>The first few trails are where the knight was pushing the wheel. You can see that the distance between them are increasing.</t>
+  </si>
+  <si>
+    <t>A vector is composed of a value for each axis. In this case, the x and y. These values can also tell us the direction, and the magnitude.</t>
   </si>
 </sst>
 </file>
@@ -861,10 +891,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D169"/>
+  <dimension ref="A1:D172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1136,26 +1166,26 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>112</v>
+      </c>
+      <c r="B30" t="s">
         <v>113</v>
-      </c>
-      <c r="B30" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>115</v>
+      </c>
+      <c r="B32" t="s">
         <v>116</v>
-      </c>
-      <c r="B32" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1192,10 +1222,10 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>106</v>
+      </c>
+      <c r="B37" t="s">
         <v>107</v>
-      </c>
-      <c r="B37" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1203,7 +1233,7 @@
         <v>105</v>
       </c>
       <c r="B38" t="s">
-        <v>106</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1363,34 +1393,34 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>117</v>
+      </c>
+      <c r="B58" s="4" t="s">
         <v>118</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>119</v>
+      </c>
+      <c r="B59" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C61">
         <v>2</v>
@@ -1398,213 +1428,247 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B62" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>123</v>
+      </c>
+      <c r="B64" s="4" t="s">
         <v>124</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>127</v>
+      </c>
+      <c r="B66" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>129</v>
+      </c>
+      <c r="B67" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>133</v>
+      </c>
+      <c r="B68" s="4" t="s">
         <v>134</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>131</v>
+      </c>
+      <c r="B69" s="4" t="s">
         <v>132</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>135</v>
+      </c>
+      <c r="B70" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>137</v>
+      </c>
+      <c r="B71" s="4" t="s">
         <v>138</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>140</v>
+      </c>
+      <c r="B73" t="s">
         <v>141</v>
-      </c>
-      <c r="B73" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>142</v>
+      </c>
+      <c r="B74" t="s">
         <v>143</v>
-      </c>
-      <c r="B74" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B75" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B76" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B77" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B78" t="s">
-        <v>149</v>
+        <v>172</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B79" t="s">
-        <v>151</v>
+        <v>173</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>148</v>
+      </c>
+      <c r="B80" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>149</v>
+      </c>
+      <c r="B81" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>160</v>
+      </c>
+      <c r="B82" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>162</v>
+      </c>
+      <c r="B83" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>163</v>
+      </c>
+      <c r="B84" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>150</v>
       </c>
-      <c r="B80" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>152</v>
-      </c>
-      <c r="B81" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>153</v>
-      </c>
-      <c r="B82" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B83" s="2"/>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B85" s="2"/>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B87" s="2"/>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B89" s="2"/>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B91" s="4"/>
-    </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B107" s="4"/>
-    </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B113" s="4"/>
-    </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B115" s="4"/>
-    </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B127" s="3"/>
-    </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B129" s="4"/>
-    </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B141" s="2"/>
-    </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B145" s="2"/>
-    </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B146" s="2"/>
-    </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B147" s="2"/>
+      <c r="B85" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>166</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>167</v>
+      </c>
+      <c r="B87" t="s">
+        <v>168</v>
+      </c>
+      <c r="C87">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B88" s="2"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B90" s="2"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B92" s="2"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B94" s="4"/>
+    </row>
+    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B110" s="4"/>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B116" s="4"/>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B118" s="4"/>
+    </row>
+    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B130" s="3"/>
+    </row>
+    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B132" s="4"/>
+    </row>
+    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B144" s="2"/>
+    </row>
+    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B148" s="2"/>
     </row>
     <row r="149" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B149" s="2"/>
@@ -1612,9 +1676,6 @@
     <row r="150" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B150" s="2"/>
     </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B151" s="2"/>
-    </row>
     <row r="152" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B152" s="2"/>
     </row>
@@ -1627,14 +1688,23 @@
     <row r="155" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B155" s="2"/>
     </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B163" s="4"/>
-    </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B164" s="4"/>
-    </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B169" s="2"/>
+    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B156" s="2"/>
+    </row>
+    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B157" s="2"/>
+    </row>
+    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B158" s="2"/>
+    </row>
+    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B166" s="4"/>
+    </row>
+    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B167" s="4"/>
+    </row>
+    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B172" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
art stuff for act 2-2
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11444EA8-FBCB-4F37-AF9B-3A774CB535F9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7472FD53-6487-4271-9AEC-64F005F4740A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="175">
   <si>
     <t>Key</t>
   </si>
@@ -439,9 +439,6 @@
     <t>Magnitude</t>
   </si>
   <si>
-    <t>Newton’s second law states that the acceleration of an object equals the net force acting on the object over the object’s mass.</t>
-  </si>
-  <si>
     <t>newton_second_law_dlg_1</t>
   </si>
   <si>
@@ -545,6 +542,9 @@
   </si>
   <si>
     <t>A vector is composed of a value for each axis. In this case, the x and y. These values can also tell us the direction, and the magnitude.</t>
+  </si>
+  <si>
+    <t>Newton's second law states that the acceleration of an object is proportional to the net force acting on it, and inversely proportional to its mass.</t>
   </si>
 </sst>
 </file>
@@ -601,7 +601,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -611,6 +611,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -893,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1233,7 +1234,7 @@
         <v>105</v>
       </c>
       <c r="B38" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1430,8 +1431,8 @@
       <c r="A62" t="s">
         <v>109</v>
       </c>
-      <c r="B62" t="s">
-        <v>139</v>
+      <c r="B62" s="5" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1452,10 +1453,10 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>156</v>
+      </c>
+      <c r="B65" s="4" t="s">
         <v>157</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -1508,130 +1509,130 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>151</v>
+      </c>
+      <c r="B72" s="4" t="s">
         <v>152</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>139</v>
+      </c>
+      <c r="B73" t="s">
         <v>140</v>
-      </c>
-      <c r="B73" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>141</v>
+      </c>
+      <c r="B74" t="s">
         <v>142</v>
-      </c>
-      <c r="B74" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B75" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B76" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B77" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B78" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B79" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B80" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B81" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>159</v>
+      </c>
+      <c r="B82" t="s">
         <v>160</v>
-      </c>
-      <c r="B82" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B83" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B84" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>149</v>
+      </c>
+      <c r="B85" t="s">
         <v>150</v>
-      </c>
-      <c r="B85" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>166</v>
+      </c>
+      <c r="B87" t="s">
         <v>167</v>
-      </c>
-      <c r="B87" t="s">
-        <v>168</v>
       </c>
       <c r="C87">
         <v>3</v>

</xml_diff>

<commit_message>
more art stuff for act 2-2, transitions, animations
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7472FD53-6487-4271-9AEC-64F005F4740A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945D55C8-417B-4599-B5AB-073F06459C2C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="179">
   <si>
     <t>Key</t>
   </si>
@@ -526,9 +526,6 @@
     <t>Targets Eliminated</t>
   </si>
   <si>
-    <t>Press this button once you are finish.</t>
-  </si>
-  <si>
     <t>At this point, the distance between each trail is equal. This means that the net force acting on the wheel equals zero.</t>
   </si>
   <si>
@@ -545,6 +542,21 @@
   </si>
   <si>
     <t>Newton's second law states that the acceleration of an object is proportional to the net force acting on it, and inversely proportional to its mass.</t>
+  </si>
+  <si>
+    <t>Press this button when you are ready to continue.</t>
+  </si>
+  <si>
+    <t>dragAngleHelp</t>
+  </si>
+  <si>
+    <t>Drag the knob to adjust the cannon's angle.</t>
+  </si>
+  <si>
+    <t>Remember to check the graph to analyze the trajectory of the cannonball.</t>
+  </si>
+  <si>
+    <t>graphReminder</t>
   </si>
 </sst>
 </file>
@@ -894,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1432,7 +1444,7 @@
         <v>109</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1552,7 +1564,7 @@
         <v>153</v>
       </c>
       <c r="B77" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -1560,7 +1572,7 @@
         <v>145</v>
       </c>
       <c r="B78" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -1568,7 +1580,7 @@
         <v>146</v>
       </c>
       <c r="B79" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -1576,7 +1588,7 @@
         <v>147</v>
       </c>
       <c r="B80" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -1584,7 +1596,7 @@
         <v>148</v>
       </c>
       <c r="B81" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -1624,7 +1636,7 @@
         <v>165</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -1639,7 +1651,20 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B88" s="2"/>
+      <c r="A88" t="s">
+        <v>175</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>178</v>
+      </c>
+      <c r="B89" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B90" s="2"/>

</xml_diff>

<commit_message>
act 2-2 dialog stuff
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945D55C8-417B-4599-B5AB-073F06459C2C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E7E7FD2-28A5-403A-959D-4FCC277C41CB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="189">
   <si>
     <t>Key</t>
   </si>
@@ -472,9 +472,6 @@
     <t>newton_second_law_dlg_9</t>
   </si>
   <si>
-    <t>The nefarious goblins have appeared out of thin air! They are surely up to no good. Get rid of them by using the wheel!</t>
-  </si>
-  <si>
     <t>examples</t>
   </si>
   <si>
@@ -557,6 +554,39 @@
   </si>
   <si>
     <t>graphReminder</t>
+  </si>
+  <si>
+    <t>newton_second_law_2_dlg_1</t>
+  </si>
+  <si>
+    <t>newton_second_law_2_dlg_2</t>
+  </si>
+  <si>
+    <t>newton_second_law_2_dlg_3</t>
+  </si>
+  <si>
+    <t>newton_second_law_2_dlg_4</t>
+  </si>
+  <si>
+    <t>Let us bring forth the mighty cannon to vanquish these vermin!</t>
+  </si>
+  <si>
+    <t>newton_second_law_2_dlg_5</t>
+  </si>
+  <si>
+    <t>In this scenario, we are applying force to a cannonball with explosion.</t>
+  </si>
+  <si>
+    <t>This short burst of force will allow the cannonball to accelerate within a fraction of a second to reach high velocity.</t>
+  </si>
+  <si>
+    <t>The nefarious goblins have appeared out of thin air! They are surely up to no good. Push them off the cliff using the wheel.</t>
+  </si>
+  <si>
+    <t>Hark! More goblins have appeared! This time, they have positioned themselves at different heights.</t>
+  </si>
+  <si>
+    <t>But fear not, we have the very tool to get the job done.</t>
   </si>
 </sst>
 </file>
@@ -906,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1246,7 +1276,7 @@
         <v>105</v>
       </c>
       <c r="B38" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1444,7 +1474,7 @@
         <v>109</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1465,10 +1495,10 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>155</v>
+      </c>
+      <c r="B65" s="4" t="s">
         <v>156</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -1521,10 +1551,10 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>150</v>
+      </c>
+      <c r="B72" s="4" t="s">
         <v>151</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -1548,7 +1578,7 @@
         <v>143</v>
       </c>
       <c r="B75" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -1556,15 +1586,15 @@
         <v>144</v>
       </c>
       <c r="B76" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B77" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -1572,7 +1602,7 @@
         <v>145</v>
       </c>
       <c r="B78" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -1580,7 +1610,7 @@
         <v>146</v>
       </c>
       <c r="B79" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -1588,7 +1618,7 @@
         <v>147</v>
       </c>
       <c r="B80" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -1596,55 +1626,55 @@
         <v>148</v>
       </c>
       <c r="B81" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>158</v>
+      </c>
+      <c r="B82" t="s">
         <v>159</v>
-      </c>
-      <c r="B82" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B83" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B84" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>149</v>
       </c>
-      <c r="B85" t="s">
-        <v>150</v>
+      <c r="B85" s="2" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>165</v>
+      </c>
+      <c r="B87" t="s">
         <v>166</v>
-      </c>
-      <c r="B87" t="s">
-        <v>167</v>
       </c>
       <c r="C87">
         <v>3</v>
@@ -1652,28 +1682,59 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>174</v>
+      </c>
+      <c r="B88" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>177</v>
+      </c>
+      <c r="B89" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>178</v>
       </c>
-      <c r="B89" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B90" s="2"/>
+      <c r="B90" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>179</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B92" s="2"/>
+      <c r="A92" t="s">
+        <v>180</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>181</v>
+      </c>
+      <c r="B93" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B94" s="4"/>
+      <c r="A94" t="s">
+        <v>183</v>
+      </c>
+      <c r="B94" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B110" s="4"/>

</xml_diff>

<commit_message>
more art assets for act 3, added simpler first level, added tutorial
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E7E7FD2-28A5-403A-959D-4FCC277C41CB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787EB250-8BEB-46D6-98DA-8CBF50A6FB3C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="197">
   <si>
     <t>Key</t>
   </si>
@@ -232,9 +232,6 @@
     <t>There are two forces currently acting on this object: gravity and normal force.</t>
   </si>
   <si>
-    <t>Gather your forces for a daring rescue!</t>
-  </si>
-  <si>
     <t>newton_first_law_inertia_dlg_1</t>
   </si>
   <si>
@@ -587,6 +584,33 @@
   </si>
   <si>
     <t>But fear not, we have the very tool to get the job done.</t>
+  </si>
+  <si>
+    <t>dragForcePushHelp</t>
+  </si>
+  <si>
+    <t>dragForceAdjustHelp</t>
+  </si>
+  <si>
+    <t>You can reposition a Force Field by dragging it.</t>
+  </si>
+  <si>
+    <t>Drag the Force Field to this surface.</t>
+  </si>
+  <si>
+    <t>playButtonHelp</t>
+  </si>
+  <si>
+    <t>Press this button to start the simulation.</t>
+  </si>
+  <si>
+    <t>trashButtonHelp</t>
+  </si>
+  <si>
+    <t>Let us summon our mighty knights for a daring rescue!</t>
+  </si>
+  <si>
+    <t>Press and hold the trash button to clear out the Force Fields.</t>
   </si>
 </sst>
 </file>
@@ -936,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,18 +1209,18 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" t="s">
         <v>80</v>
-      </c>
-      <c r="B27" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" t="s">
         <v>82</v>
-      </c>
-      <c r="B28" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1209,82 +1233,82 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>111</v>
+      </c>
+      <c r="B30" t="s">
         <v>112</v>
-      </c>
-      <c r="B30" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>114</v>
+      </c>
+      <c r="B32" t="s">
         <v>115</v>
-      </c>
-      <c r="B32" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" t="s">
         <v>90</v>
-      </c>
-      <c r="B33" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B35" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B36" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>105</v>
+      </c>
+      <c r="B37" t="s">
         <v>106</v>
-      </c>
-      <c r="B37" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B38" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>96</v>
+      </c>
+      <c r="B39" t="s">
         <v>97</v>
-      </c>
-      <c r="B39" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1348,87 +1372,87 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>70</v>
+        <v>195</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B48" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B49" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>74</v>
+      </c>
+      <c r="B52" t="s">
         <v>75</v>
-      </c>
-      <c r="B52" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B55" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>94</v>
+      </c>
+      <c r="B57" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="C57">
         <v>4</v>
@@ -1436,34 +1460,34 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>116</v>
+      </c>
+      <c r="B58" s="4" t="s">
         <v>117</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>118</v>
+      </c>
+      <c r="B59" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C61">
         <v>2</v>
@@ -1471,210 +1495,210 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>122</v>
+      </c>
+      <c r="B64" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>154</v>
+      </c>
+      <c r="B65" s="4" t="s">
         <v>155</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>126</v>
+      </c>
+      <c r="B66" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>128</v>
+      </c>
+      <c r="B67" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>132</v>
+      </c>
+      <c r="B68" s="4" t="s">
         <v>133</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>130</v>
+      </c>
+      <c r="B69" s="4" t="s">
         <v>131</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>134</v>
+      </c>
+      <c r="B70" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>136</v>
+      </c>
+      <c r="B71" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>149</v>
+      </c>
+      <c r="B72" s="4" t="s">
         <v>150</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>138</v>
+      </c>
+      <c r="B73" t="s">
         <v>139</v>
-      </c>
-      <c r="B73" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>140</v>
+      </c>
+      <c r="B74" t="s">
         <v>141</v>
-      </c>
-      <c r="B74" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B75" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B76" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B77" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B78" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B79" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B80" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B81" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>157</v>
+      </c>
+      <c r="B82" t="s">
         <v>158</v>
-      </c>
-      <c r="B82" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B83" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B84" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>164</v>
+      </c>
+      <c r="B87" t="s">
         <v>165</v>
-      </c>
-      <c r="B87" t="s">
-        <v>166</v>
       </c>
       <c r="C87">
         <v>3</v>
@@ -1682,61 +1706,99 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>173</v>
+      </c>
+      <c r="B88" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B89" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B90" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B93" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B94" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>188</v>
+      </c>
+      <c r="B95" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>189</v>
+      </c>
+      <c r="B96" t="s">
+        <v>190</v>
+      </c>
+      <c r="C96">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>192</v>
+      </c>
+      <c r="B97" t="s">
+        <v>193</v>
+      </c>
+      <c r="C97">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>194</v>
+      </c>
+      <c r="B98" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B110" s="4"/>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
title scene art asset/setup
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E3BD05-C6BA-4608-81DC-0BE91808C5BE}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8CFF82-99B3-430F-92CE-94904D906DB8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -628,9 +628,6 @@
     <t>As you fire away, observe that the projectile will move at a constant velocity along the X-axis as it gradually falls down.</t>
   </si>
   <si>
-    <t>Mighty Force Knights: Newton's Law 1 and 2</t>
-  </si>
-  <si>
     <t>begin</t>
   </si>
   <si>
@@ -653,6 +650,9 @@
   </si>
   <si>
     <t>The Golden Ball</t>
+  </si>
+  <si>
+    <t>Mighty Force Knights\n&lt;size=30&gt;Newton's Law 1 and 2&lt;/size&gt;</t>
   </si>
 </sst>
 </file>
@@ -1002,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A105" sqref="A105"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,7 +1047,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1146,26 +1146,26 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>204</v>
+      </c>
+      <c r="B15" t="s">
         <v>205</v>
-      </c>
-      <c r="B15" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>206</v>
+      </c>
+      <c r="B16" t="s">
         <v>207</v>
-      </c>
-      <c r="B16" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>202</v>
+      </c>
+      <c r="B17" t="s">
         <v>203</v>
-      </c>
-      <c r="B17" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1899,10 +1899,10 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
+        <v>208</v>
+      </c>
+      <c r="B105" t="s">
         <v>209</v>
-      </c>
-      <c r="B105" t="s">
-        <v>210</v>
       </c>
       <c r="C105">
         <v>2</v>

</xml_diff>

<commit_message>
act 3 end, ending stuff
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8CFF82-99B3-430F-92CE-94904D906DB8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC7604B-413A-4359-8045-3AF2CCC4325C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="219">
   <si>
     <t>Key</t>
   </si>
@@ -538,9 +538,6 @@
     <t>dragAngleHelp</t>
   </si>
   <si>
-    <t>Drag the knob to adjust the cannon's angle.</t>
-  </si>
-  <si>
     <t>Remember to check the graph to analyze the trajectory of the cannonball.</t>
   </si>
   <si>
@@ -553,9 +550,6 @@
     <t>newton_second_law_2_dlg_3</t>
   </si>
   <si>
-    <t>newton_second_law_2_dlg_4</t>
-  </si>
-  <si>
     <t>Let us bring forth the mighty cannon to vanquish these vermin!</t>
   </si>
   <si>
@@ -622,12 +616,6 @@
     <t>Beware! More goblins have appeared!</t>
   </si>
   <si>
-    <t>The cannon will apply a short burst of force to allow the projectile to fly far.</t>
-  </si>
-  <si>
-    <t>As you fire away, observe that the projectile will move at a constant velocity along the X-axis as it gradually falls down.</t>
-  </si>
-  <si>
     <t>begin</t>
   </si>
   <si>
@@ -653,6 +641,42 @@
   </si>
   <si>
     <t>Mighty Force Knights\n&lt;size=30&gt;Newton's Law 1 and 2&lt;/size&gt;</t>
+  </si>
+  <si>
+    <t>act_2_end_dlg_1</t>
+  </si>
+  <si>
+    <t>Drag this to adjust the cannon's angle.</t>
+  </si>
+  <si>
+    <t>As you fire away, observe that the projectile will move at a constant velocity along the X-axis.</t>
+  </si>
+  <si>
+    <t>act_2_end_dlg_2</t>
+  </si>
+  <si>
+    <t>A large meteorite is approaching Earth! It will surely cause a disaster of epic proportion across the globe!</t>
+  </si>
+  <si>
+    <t>Seek the golden ball, for it will grant you the force to thwart the approaching doom.</t>
+  </si>
+  <si>
+    <t>end_title</t>
+  </si>
+  <si>
+    <t>end_desc</t>
+  </si>
+  <si>
+    <t>Thank you for playing!</t>
+  </si>
+  <si>
+    <t>GAME COMPLETE</t>
+  </si>
+  <si>
+    <t>finish</t>
+  </si>
+  <si>
+    <t>FINISH</t>
   </si>
 </sst>
 </file>
@@ -1000,10 +1024,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D178"/>
+  <dimension ref="A1:D176"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,7 +1071,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1146,34 +1170,34 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B15" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B16" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B17" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B18" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1208,7 +1232,7 @@
         <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C22">
         <v>3</v>
@@ -1216,10 +1240,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B23" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C23">
         <v>1.5</v>
@@ -1227,10 +1251,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B24" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C24">
         <v>1.5</v>
@@ -1238,10 +1262,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B25" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C25">
         <v>1.5</v>
@@ -1479,7 +1503,7 @@
         <v>44</v>
       </c>
       <c r="B54" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1789,7 +1813,7 @@
         <v>146</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -1816,31 +1840,31 @@
         <v>171</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>172</v>
+        <v>208</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B96" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B97" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>175</v>
+      </c>
+      <c r="B98" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -1848,7 +1872,7 @@
         <v>177</v>
       </c>
       <c r="B99" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -1856,23 +1880,26 @@
         <v>179</v>
       </c>
       <c r="B100" t="s">
-        <v>201</v>
+        <v>182</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
+        <v>180</v>
+      </c>
+      <c r="B101" t="s">
         <v>181</v>
       </c>
-      <c r="B101" t="s">
-        <v>184</v>
+      <c r="C101">
+        <v>3</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B102" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C102">
         <v>3</v>
@@ -1883,58 +1910,99 @@
         <v>185</v>
       </c>
       <c r="B103" t="s">
-        <v>186</v>
-      </c>
-      <c r="C103">
-        <v>3</v>
+        <v>187</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>187</v>
+        <v>204</v>
       </c>
       <c r="B104" t="s">
-        <v>189</v>
+        <v>205</v>
+      </c>
+      <c r="C104">
+        <v>2</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B105" t="s">
-        <v>209</v>
-      </c>
-      <c r="C105">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>210</v>
+      </c>
+      <c r="B106" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>213</v>
+      </c>
+      <c r="B107" t="s">
+        <v>216</v>
+      </c>
+      <c r="C107">
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B116" s="4"/>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>214</v>
+      </c>
+      <c r="B108" t="s">
+        <v>215</v>
+      </c>
+      <c r="C108">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>217</v>
+      </c>
+      <c r="B109" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B114" s="4"/>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B120" s="4"/>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B122" s="4"/>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B124" s="4"/>
+    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B134" s="3"/>
     </row>
     <row r="136" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B136" s="3"/>
-    </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B138" s="4"/>
-    </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B150" s="2"/>
+      <c r="B136" s="4"/>
+    </row>
+    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B148" s="2"/>
+    </row>
+    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B152" s="2"/>
+    </row>
+    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B153" s="2"/>
     </row>
     <row r="154" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B154" s="2"/>
     </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B155" s="2"/>
-    </row>
     <row r="156" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B156" s="2"/>
     </row>
+    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B157" s="2"/>
+    </row>
     <row r="158" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B158" s="2"/>
     </row>
@@ -1950,20 +2018,14 @@
     <row r="162" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B162" s="2"/>
     </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B163" s="2"/>
-    </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B164" s="2"/>
-    </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B172" s="4"/>
-    </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B173" s="4"/>
-    </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B178" s="2"/>
+    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B170" s="4"/>
+    </row>
+    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B171" s="4"/>
+    </row>
+    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B176" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
bunch of tweaks and fixes, added build
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4907B2B-B157-4F59-A884-8024C4B4491A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF090D8-64F1-45EE-AA0A-06E2C3202515}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -625,9 +625,6 @@
     <t>Thank you for playing!</t>
   </si>
   <si>
-    <t>GAME COMPLETE</t>
-  </si>
-  <si>
     <t>finish</t>
   </si>
   <si>
@@ -683,6 +680,9 @@
   </si>
   <si>
     <t>0 Net Force (Balanced)</t>
+  </si>
+  <si>
+    <t>GLORY IS YOURS</t>
   </si>
 </sst>
 </file>
@@ -1032,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1365,7 +1365,7 @@
         <v>60</v>
       </c>
       <c r="B36" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1477,7 +1477,7 @@
         <v>40</v>
       </c>
       <c r="B50" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1493,7 +1493,7 @@
         <v>42</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1525,7 +1525,7 @@
         <v>66</v>
       </c>
       <c r="B56" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1533,7 +1533,7 @@
         <v>67</v>
       </c>
       <c r="B57" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1557,7 +1557,7 @@
         <v>77</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1565,7 +1565,7 @@
         <v>78</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1573,7 +1573,7 @@
         <v>79</v>
       </c>
       <c r="B62" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1581,7 +1581,7 @@
         <v>80</v>
       </c>
       <c r="B63" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1597,10 +1597,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>210</v>
+      </c>
+      <c r="B65" s="4" t="s">
         <v>211</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1771,7 +1771,7 @@
         <v>133</v>
       </c>
       <c r="B86" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -1787,7 +1787,7 @@
         <v>135</v>
       </c>
       <c r="B88" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -1795,7 +1795,7 @@
         <v>136</v>
       </c>
       <c r="B89" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -1827,7 +1827,7 @@
         <v>137</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -1943,7 +1943,7 @@
         <v>194</v>
       </c>
       <c r="B106" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -1951,7 +1951,7 @@
         <v>197</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -1959,7 +1959,7 @@
         <v>198</v>
       </c>
       <c r="B108" t="s">
-        <v>201</v>
+        <v>220</v>
       </c>
       <c r="C108">
         <v>2</v>
@@ -1978,10 +1978,10 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
+        <v>201</v>
+      </c>
+      <c r="B110" t="s">
         <v>202</v>
-      </c>
-      <c r="B110" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
initial revision of act 1-1
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF090D8-64F1-45EE-AA0A-06E2C3202515}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB5B65B-905A-4BA9-9FDD-3C7BD283FBD1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="223">
   <si>
     <t>Key</t>
   </si>
@@ -184,9 +184,6 @@
     <t>forceNormal</t>
   </si>
   <si>
-    <t>Force Normal</t>
-  </si>
-  <si>
     <t>newton_first_law_dlg_3_2</t>
   </si>
   <si>
@@ -683,6 +680,15 @@
   </si>
   <si>
     <t>GLORY IS YOURS</t>
+  </si>
+  <si>
+    <t>netForce</t>
+  </si>
+  <si>
+    <t>Net Force</t>
+  </si>
+  <si>
+    <t>Force Ground</t>
   </si>
 </sst>
 </file>
@@ -1030,10 +1036,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D177"/>
+  <dimension ref="A1:D178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="B108" sqref="B108"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,7 +1083,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1176,34 +1182,34 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>186</v>
+      </c>
+      <c r="B15" t="s">
         <v>187</v>
-      </c>
-      <c r="B15" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>188</v>
+      </c>
+      <c r="B16" t="s">
         <v>189</v>
-      </c>
-      <c r="B16" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>184</v>
+      </c>
+      <c r="B17" t="s">
         <v>185</v>
-      </c>
-      <c r="B17" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>181</v>
+      </c>
+      <c r="B18" t="s">
         <v>182</v>
-      </c>
-      <c r="B18" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1238,7 +1244,7 @@
         <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C22">
         <v>3</v>
@@ -1246,10 +1252,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>175</v>
+      </c>
+      <c r="B23" t="s">
         <v>176</v>
-      </c>
-      <c r="B23" t="s">
-        <v>177</v>
       </c>
       <c r="C23">
         <v>1.5</v>
@@ -1257,10 +1263,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>177</v>
+      </c>
+      <c r="B24" t="s">
         <v>178</v>
-      </c>
-      <c r="B24" t="s">
-        <v>179</v>
       </c>
       <c r="C24">
         <v>1.5</v>
@@ -1268,10 +1274,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>179</v>
+      </c>
+      <c r="B25" t="s">
         <v>180</v>
-      </c>
-      <c r="B25" t="s">
-        <v>181</v>
       </c>
       <c r="C25">
         <v>1.5</v>
@@ -1314,18 +1320,18 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" t="s">
         <v>56</v>
-      </c>
-      <c r="B30" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" t="s">
         <v>58</v>
-      </c>
-      <c r="B31" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1341,95 +1347,95 @@
         <v>53</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
+        <v>222</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" t="s">
         <v>72</v>
-      </c>
-      <c r="B34" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" t="s">
         <v>74</v>
-      </c>
-      <c r="B35" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B36" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>99</v>
+      </c>
+      <c r="B37" t="s">
         <v>100</v>
-      </c>
-      <c r="B37" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>102</v>
+      </c>
+      <c r="B39" t="s">
         <v>103</v>
-      </c>
-      <c r="B39" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>81</v>
+        <v>220</v>
       </c>
       <c r="B40" t="s">
-        <v>82</v>
+        <v>221</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B41" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B42" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B43" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B44" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1437,226 +1443,226 @@
         <v>93</v>
       </c>
       <c r="B45" t="s">
-        <v>145</v>
+        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B46" t="s">
-        <v>86</v>
+        <v>144</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>37</v>
+        <v>84</v>
       </c>
       <c r="B47" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>37</v>
+      </c>
+      <c r="B48" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>50</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>39</v>
+      </c>
+      <c r="B50" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>40</v>
+      </c>
+      <c r="B51" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>39</v>
-      </c>
-      <c r="B49" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>42</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>43</v>
+      </c>
+      <c r="B54" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>44</v>
+      </c>
+      <c r="B55" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>40</v>
-      </c>
-      <c r="B50" t="s">
+      <c r="B56" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>65</v>
+      </c>
+      <c r="B57" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>55</v>
-      </c>
-      <c r="B51" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>42</v>
-      </c>
-      <c r="B52" s="3" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>66</v>
+      </c>
+      <c r="B58" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>43</v>
-      </c>
-      <c r="B53" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>44</v>
-      </c>
-      <c r="B54" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>65</v>
-      </c>
-      <c r="B55" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>67</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>68</v>
+      </c>
+      <c r="B60" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>66</v>
-      </c>
-      <c r="B56" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>67</v>
-      </c>
-      <c r="B57" t="s">
+      <c r="B61" s="3" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>68</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>69</v>
-      </c>
-      <c r="B59" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>77</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B62" s="2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>78</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B63" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>79</v>
       </c>
-      <c r="B62" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>80</v>
-      </c>
-      <c r="B63" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>83</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C64">
-        <v>4</v>
+      <c r="B64" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>210</v>
+        <v>82</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>211</v>
+        <v>83</v>
+      </c>
+      <c r="C65">
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>105</v>
+        <v>209</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>106</v>
+        <v>210</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>96</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C69">
-        <v>2</v>
+        <v>108</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>95</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B70" s="5" t="s">
-        <v>157</v>
+      <c r="C70">
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>110</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>113</v>
+        <v>96</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>112</v>
@@ -1664,95 +1670,95 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>143</v>
+        <v>110</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>144</v>
+        <v>111</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>116</v>
+        <v>143</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>127</v>
-      </c>
-      <c r="B81" t="s">
-        <v>128</v>
+        <v>137</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B82" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B83" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B84" t="s">
         <v>141</v>
@@ -1760,160 +1766,157 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>131</v>
+      </c>
+      <c r="B85" t="s">
         <v>140</v>
-      </c>
-      <c r="B85" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B86" t="s">
-        <v>213</v>
+        <v>155</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B87" t="s">
-        <v>155</v>
+        <v>212</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B88" t="s">
-        <v>214</v>
+        <v>154</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B89" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="B90" t="s">
-        <v>147</v>
+        <v>214</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B91" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
+        <v>147</v>
+      </c>
+      <c r="B92" t="s">
         <v>149</v>
-      </c>
-      <c r="B92" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>137</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>216</v>
+        <v>148</v>
+      </c>
+      <c r="B93" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>158</v>
+        <v>215</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>153</v>
-      </c>
-      <c r="B95" t="s">
-        <v>154</v>
-      </c>
-      <c r="C95">
-        <v>3</v>
+        <v>151</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>159</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>195</v>
+        <v>152</v>
+      </c>
+      <c r="B96" t="s">
+        <v>153</v>
+      </c>
+      <c r="C96">
+        <v>3</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>161</v>
-      </c>
-      <c r="B97" t="s">
-        <v>160</v>
+        <v>158</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B98" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>163</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
+      </c>
+      <c r="B99" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>165</v>
-      </c>
-      <c r="B100" t="s">
-        <v>196</v>
+        <v>162</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B101" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B102" t="s">
         <v>168</v>
       </c>
-      <c r="C102">
-        <v>3</v>
-      </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B103" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C103">
         <v>3</v>
@@ -1921,89 +1924,97 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B104" t="s">
-        <v>174</v>
+        <v>170</v>
+      </c>
+      <c r="C104">
+        <v>3</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="B105" t="s">
-        <v>192</v>
-      </c>
-      <c r="C105">
-        <v>2</v>
+        <v>173</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B106" t="s">
-        <v>217</v>
+        <v>191</v>
+      </c>
+      <c r="C106">
+        <v>2</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>197</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>218</v>
+        <v>193</v>
+      </c>
+      <c r="B107" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>198</v>
-      </c>
-      <c r="B108" t="s">
-        <v>220</v>
-      </c>
-      <c r="C108">
-        <v>2</v>
+        <v>196</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B109" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="C109">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
+        <v>198</v>
+      </c>
+      <c r="B110" t="s">
+        <v>199</v>
+      </c>
+      <c r="C110">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>200</v>
+      </c>
+      <c r="B111" t="s">
         <v>201</v>
       </c>
-      <c r="B110" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B115" s="4"/>
-    </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B121" s="4"/>
-    </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B123" s="4"/>
-    </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B135" s="3"/>
-    </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B137" s="4"/>
-    </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B149" s="2"/>
-    </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B153" s="2"/>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B116" s="4"/>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B122" s="4"/>
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B124" s="4"/>
+    </row>
+    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B136" s="3"/>
+    </row>
+    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B138" s="4"/>
+    </row>
+    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B150" s="2"/>
     </row>
     <row r="154" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B154" s="2"/>
@@ -2011,8 +2022,8 @@
     <row r="155" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B155" s="2"/>
     </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B157" s="2"/>
+    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B156" s="2"/>
     </row>
     <row r="158" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B158" s="2"/>
@@ -2032,14 +2043,17 @@
     <row r="163" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B163" s="2"/>
     </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B171" s="4"/>
+    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B164" s="2"/>
     </row>
     <row r="172" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B172" s="4"/>
     </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B177" s="2"/>
+    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B173" s="4"/>
+    </row>
+    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B178" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update dialogs in act 1-1, more tweaks
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB5B65B-905A-4BA9-9FDD-3C7BD283FBD1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC846D5-1E39-4630-806B-CAB8434BF00C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="221">
   <si>
     <t>Key</t>
   </si>
@@ -139,24 +139,6 @@
     <t>newton_first_law_desc</t>
   </si>
   <si>
-    <t>newton_first_law_dlg_2</t>
-  </si>
-  <si>
-    <t>newton_first_law_dlg_3</t>
-  </si>
-  <si>
-    <t>It looks like the princess has been taken hostage by these nefarious goblins!</t>
-  </si>
-  <si>
-    <t>newton_first_law_dlg_4</t>
-  </si>
-  <si>
-    <t>newton_first_law_dlg_5</t>
-  </si>
-  <si>
-    <t>newton_first_law_dlg_6</t>
-  </si>
-  <si>
     <t>velocityX</t>
   </si>
   <si>
@@ -172,9 +154,6 @@
     <t>Newton's first law states that an object at rest will remain at rest, and an object in motion will maintain a constant velocity unless acted upon by a net external force.</t>
   </si>
   <si>
-    <t>newton_first_law_dlg_1_2</t>
-  </si>
-  <si>
     <t>forceGravity</t>
   </si>
   <si>
@@ -184,9 +163,6 @@
     <t>forceNormal</t>
   </si>
   <si>
-    <t>newton_first_law_dlg_3_2</t>
-  </si>
-  <si>
     <t>newton_balanced_force</t>
   </si>
   <si>
@@ -202,39 +178,6 @@
     <t>forceZeroNetForce</t>
   </si>
   <si>
-    <t>A net external force is the sum of all forces acting on the object. If the net external force is zero, then there is no acceleration.</t>
-  </si>
-  <si>
-    <t>I will now drop a large object from the sky to demonstrate.</t>
-  </si>
-  <si>
-    <t>The normal force is pushing the object outwards from the surface.</t>
-  </si>
-  <si>
-    <t>There are two forces currently acting on this object: gravity and normal force.</t>
-  </si>
-  <si>
-    <t>newton_first_law_inertia_dlg_1</t>
-  </si>
-  <si>
-    <t>newton_first_law_inertia_dlg_2</t>
-  </si>
-  <si>
-    <t>newton_first_law_inertia_dlg_3</t>
-  </si>
-  <si>
-    <t>newton_first_law_inertia_dlg_4</t>
-  </si>
-  <si>
-    <t>newton_first_law_inertia_dlg_5</t>
-  </si>
-  <si>
-    <t>I will now drop another object from the sky. This time with less mass. Just one more block to rescue our damsel in distress!</t>
-  </si>
-  <si>
-    <t>Inertia is the tendency of any physical object to resist any change in motion. A change in motion is acceleration due to net force acting on the object.</t>
-  </si>
-  <si>
     <t>forceFriction</t>
   </si>
   <si>
@@ -247,9 +190,6 @@
     <t>Force Push</t>
   </si>
   <si>
-    <t>Excellent! Notice how it took a couple of knights to push the block?</t>
-  </si>
-  <si>
     <t>newton_first_law_inertia_2_dlg_1</t>
   </si>
   <si>
@@ -538,9 +478,6 @@
     <t>trashButtonHelp</t>
   </si>
   <si>
-    <t>Let us summon our mighty knights for a daring rescue!</t>
-  </si>
-  <si>
     <t>Press and hold the trash button to clear out the Force Fields.</t>
   </si>
   <si>
@@ -628,18 +565,6 @@
     <t>FINISH</t>
   </si>
   <si>
-    <t>The gravity force is pulling the object towards Earth, which allows it to fall in the first place.</t>
-  </si>
-  <si>
-    <t>The block's mass allows its frictional force to resist the pushing force of the knights.</t>
-  </si>
-  <si>
-    <t>Adding both the gravity and normal force will result in zero net force. Thus, the object is at rest.</t>
-  </si>
-  <si>
-    <t>Mass is a measure of inertia. The unit of measurement shown here is in kg (kilograms), which is 1000 grams per 1 kilogram.</t>
-  </si>
-  <si>
     <t>In this scenario, we will learn more about how inertia influences force.</t>
   </si>
   <si>
@@ -689,6 +614,75 @@
   </si>
   <si>
     <t>Force Ground</t>
+  </si>
+  <si>
+    <t>newton_first_law_dlg_kidnap_1</t>
+  </si>
+  <si>
+    <t>newton_first_law_dlg_kidnap_2</t>
+  </si>
+  <si>
+    <t>Oh no! The princess has been taken hostage by these nefarious goblins!</t>
+  </si>
+  <si>
+    <t>Let me drop an object that will help us in this predicament. This will show us the first law in action.</t>
+  </si>
+  <si>
+    <t>newton_first_law_dlg_gravity</t>
+  </si>
+  <si>
+    <t>The gravity force is pulling the object towards Earth, which allows it to fall.</t>
+  </si>
+  <si>
+    <t>Now that the object has landed, the ground is pushing it up. This cancels out the gravity force. The object is now at rest.</t>
+  </si>
+  <si>
+    <t>newton_first_law_dlg_landed_1</t>
+  </si>
+  <si>
+    <t>newton_first_law_dlg_landed_2</t>
+  </si>
+  <si>
+    <t>Go ahead and summon a mighty knight to push the object!</t>
+  </si>
+  <si>
+    <t>newton_first_law_dlg_goblins_1</t>
+  </si>
+  <si>
+    <t>The goblins are pushing back! This cancels out the knight's push.</t>
+  </si>
+  <si>
+    <t>This means that an object will keep doing what it is doing, be it sitting or moving, until it is bothered by a bunch of forces (net force).</t>
+  </si>
+  <si>
+    <t>newton_first_law_dlg_goblins_2</t>
+  </si>
+  <si>
+    <t>Summon more knights to overcome the goblins on the other side!</t>
+  </si>
+  <si>
+    <t>newton_first_law_dlg_next_1</t>
+  </si>
+  <si>
+    <t>Excellent! As you can see, the side with more force will determine the direction of the net force acting on the object.</t>
+  </si>
+  <si>
+    <t>newton_first_law_dlg_next_2</t>
+  </si>
+  <si>
+    <t>We need one more block to rescue our damsel in distress!</t>
+  </si>
+  <si>
+    <t>newton_first_law_dlg_block2_1</t>
+  </si>
+  <si>
+    <t>newton_first_law_dlg_block2_2</t>
+  </si>
+  <si>
+    <t>We have enough knights to overcome this force. Summon the mighty knights for this one last push!</t>
+  </si>
+  <si>
+    <t>This block has no wheels. The force of friction will allow the block to resist a certain amount of push or pull from all sides.</t>
   </si>
 </sst>
 </file>
@@ -1036,10 +1030,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D178"/>
+  <dimension ref="A1:D177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,7 +1077,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1182,34 +1176,34 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="B15" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="B16" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="B17" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
       <c r="B18" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1225,18 +1219,18 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1244,7 +1238,7 @@
         <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="C22">
         <v>3</v>
@@ -1252,10 +1246,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>175</v>
+        <v>154</v>
       </c>
       <c r="B23" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="C23">
         <v>1.5</v>
@@ -1263,10 +1257,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
       <c r="B24" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="C24">
         <v>1.5</v>
@@ -1274,10 +1268,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="B25" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="C25">
         <v>1.5</v>
@@ -1299,7 +1293,7 @@
         <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1320,146 +1314,146 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>222</v>
+        <v>197</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="B34" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="B35" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B36" t="s">
-        <v>218</v>
+        <v>193</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="B37" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="B38" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="B39" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>220</v>
+        <v>195</v>
       </c>
       <c r="B40" t="s">
-        <v>221</v>
+        <v>196</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="B41" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="B42" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="B43" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="B44" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="B45" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="B46" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="B47" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1467,456 +1461,459 @@
         <v>37</v>
       </c>
       <c r="B48" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>198</v>
       </c>
       <c r="B49" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>39</v>
+        <v>199</v>
       </c>
       <c r="B50" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>202</v>
+      </c>
+      <c r="B51" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>205</v>
+      </c>
+      <c r="B52" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>206</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>208</v>
+      </c>
+      <c r="B54" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>211</v>
+      </c>
+      <c r="B55" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>213</v>
+      </c>
+      <c r="B56" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>215</v>
+      </c>
+      <c r="B57" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>217</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>218</v>
+      </c>
+      <c r="B59" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>56</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>57</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>58</v>
+      </c>
+      <c r="B62" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>59</v>
+      </c>
+      <c r="B63" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>62</v>
+      </c>
+      <c r="B64" s="4" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>40</v>
-      </c>
-      <c r="B51" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>54</v>
-      </c>
-      <c r="B52" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>42</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>43</v>
-      </c>
-      <c r="B54" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>44</v>
-      </c>
-      <c r="B55" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>64</v>
-      </c>
-      <c r="B56" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>65</v>
-      </c>
-      <c r="B57" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>66</v>
-      </c>
-      <c r="B58" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>67</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>68</v>
-      </c>
-      <c r="B60" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>76</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>77</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>78</v>
-      </c>
-      <c r="B63" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>79</v>
-      </c>
-      <c r="B64" t="s">
-        <v>211</v>
+      <c r="C64">
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>82</v>
+        <v>184</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C65">
-        <v>4</v>
+        <v>185</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>209</v>
+        <v>84</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>210</v>
+        <v>85</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>108</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>113</v>
+        <v>75</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C69">
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>95</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C70">
-        <v>2</v>
+        <v>76</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>96</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>156</v>
+        <v>89</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>142</v>
+        <v>94</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>143</v>
+        <v>95</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>137</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>138</v>
+        <v>106</v>
+      </c>
+      <c r="B81" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="B82" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="B83" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="B84" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="B85" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>139</v>
+        <v>112</v>
       </c>
       <c r="B86" t="s">
-        <v>155</v>
+        <v>187</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="B87" t="s">
-        <v>212</v>
+        <v>134</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="B88" t="s">
-        <v>154</v>
+        <v>188</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="B89" t="s">
-        <v>213</v>
+        <v>189</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="B90" t="s">
-        <v>214</v>
+        <v>126</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="B91" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="B92" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>148</v>
-      </c>
-      <c r="B93" t="s">
-        <v>150</v>
+        <v>116</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>215</v>
+        <v>137</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>151</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>157</v>
+        <v>132</v>
+      </c>
+      <c r="B95" t="s">
+        <v>133</v>
+      </c>
+      <c r="C95">
+        <v>3</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>152</v>
-      </c>
-      <c r="B96" t="s">
-        <v>153</v>
-      </c>
-      <c r="C96">
-        <v>3</v>
+        <v>138</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>158</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>194</v>
+        <v>140</v>
+      </c>
+      <c r="B97" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="B98" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>161</v>
-      </c>
-      <c r="B99" t="s">
-        <v>183</v>
+        <v>142</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>162</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>163</v>
+        <v>144</v>
+      </c>
+      <c r="B100" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="B101" t="s">
-        <v>195</v>
+        <v>148</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="B102" t="s">
-        <v>168</v>
+        <v>147</v>
+      </c>
+      <c r="C102">
+        <v>3</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="B103" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="C103">
         <v>3</v>
@@ -1924,97 +1921,89 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="B104" t="s">
-        <v>170</v>
-      </c>
-      <c r="C104">
-        <v>3</v>
+        <v>152</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B105" t="s">
-        <v>173</v>
+        <v>170</v>
+      </c>
+      <c r="C105">
+        <v>2</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="B106" t="s">
         <v>191</v>
       </c>
-      <c r="C106">
-        <v>2</v>
-      </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>193</v>
-      </c>
-      <c r="B107" t="s">
-        <v>216</v>
+        <v>175</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>196</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>217</v>
+        <v>176</v>
+      </c>
+      <c r="B108" t="s">
+        <v>194</v>
+      </c>
+      <c r="C108">
+        <v>2</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="B109" t="s">
-        <v>219</v>
+        <v>178</v>
       </c>
       <c r="C109">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
       <c r="B110" t="s">
-        <v>199</v>
-      </c>
-      <c r="C110">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>200</v>
-      </c>
-      <c r="B111" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B116" s="4"/>
-    </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B122" s="4"/>
-    </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B124" s="4"/>
-    </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B136" s="3"/>
-    </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B138" s="4"/>
-    </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B150" s="2"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B115" s="4"/>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B121" s="4"/>
+    </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B123" s="4"/>
+    </row>
+    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B135" s="3"/>
+    </row>
+    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B137" s="4"/>
+    </row>
+    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B149" s="2"/>
+    </row>
+    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B153" s="2"/>
     </row>
     <row r="154" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B154" s="2"/>
@@ -2022,8 +2011,8 @@
     <row r="155" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B155" s="2"/>
     </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B156" s="2"/>
+    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B157" s="2"/>
     </row>
     <row r="158" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B158" s="2"/>
@@ -2043,17 +2032,14 @@
     <row r="163" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B163" s="2"/>
     </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B164" s="2"/>
+    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B171" s="4"/>
     </row>
     <row r="172" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B172" s="4"/>
     </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B173" s="4"/>
-    </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B178" s="2"/>
+    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B177" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added hint system for act 3
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC846D5-1E39-4630-806B-CAB8434BF00C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A221DF47-7AB7-4373-A7F8-B2798C08CBDD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="223">
   <si>
     <t>Key</t>
   </si>
@@ -683,6 +683,12 @@
   </si>
   <si>
     <t>This block has no wheels. The force of friction will allow the block to resist a certain amount of push or pull from all sides.</t>
+  </si>
+  <si>
+    <t>hintTooltip</t>
+  </si>
+  <si>
+    <t>Press this button to show hints.</t>
   </si>
 </sst>
 </file>
@@ -1032,8 +1038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1984,6 +1990,14 @@
         <v>180</v>
       </c>
     </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>221</v>
+      </c>
+      <c r="B111" t="s">
+        <v>222</v>
+      </c>
+    </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B115" s="4"/>
     </row>

</xml_diff>

<commit_message>
moved inertia description to act 1-2
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A221DF47-7AB7-4373-A7F8-B2798C08CBDD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F345774-E672-40BC-A0BB-739C22E558BC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="231">
   <si>
     <t>Key</t>
   </si>
@@ -565,9 +565,6 @@
     <t>FINISH</t>
   </si>
   <si>
-    <t>In this scenario, we will learn more about how inertia influences force.</t>
-  </si>
-  <si>
     <t>Observe how the forces are interacting on this balance scale.</t>
   </si>
   <si>
@@ -580,9 +577,6 @@
     <t>Drag these weights on top of the platform.</t>
   </si>
   <si>
-    <t>Here's a locked treasure as a demonstration. Put the correct amount of weight on the other platform to unlock it.</t>
-  </si>
-  <si>
     <t>A mighty knight has brought us a wheel to demonstrate. The wheel is enchanted with magical trails to allow us to observe its motion.</t>
   </si>
   <si>
@@ -689,6 +683,36 @@
   </si>
   <si>
     <t>Press this button to show hints.</t>
+  </si>
+  <si>
+    <t>Here's a locked treasure chest as a demonstration. Put the correct amount of weight on the other platform to unlock it.</t>
+  </si>
+  <si>
+    <t>In this scenario, we will learn more about inertia.</t>
+  </si>
+  <si>
+    <t>newton_first_law_inertia_2_dlg_1_a</t>
+  </si>
+  <si>
+    <t>newton_first_law_inertia_2_dlg_1_b</t>
+  </si>
+  <si>
+    <t>mass_inertia</t>
+  </si>
+  <si>
+    <t>Mass = Inertia</t>
+  </si>
+  <si>
+    <t>weight_gravity</t>
+  </si>
+  <si>
+    <t>Weight = Force of Gravity</t>
+  </si>
+  <si>
+    <t>Mass is a measure of inertia. It tells us how much resistance an object has in changing motion.</t>
+  </si>
+  <si>
+    <t>The weight of an object is essentially the force of gravity.</t>
   </si>
 </sst>
 </file>
@@ -1036,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D177"/>
+  <dimension ref="A1:D181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="B111" sqref="B111"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1347,7 +1371,7 @@
         <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1371,7 +1395,7 @@
         <v>51</v>
       </c>
       <c r="B36" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1400,10 +1424,10 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B40" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1464,567 +1488,590 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>225</v>
+      </c>
+      <c r="B48" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>227</v>
+      </c>
+      <c r="B49" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>37</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B50" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>196</v>
+      </c>
+      <c r="B51" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>197</v>
+      </c>
+      <c r="B52" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>200</v>
+      </c>
+      <c r="B53" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>203</v>
+      </c>
+      <c r="B54" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>204</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>206</v>
+      </c>
+      <c r="B56" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>209</v>
+      </c>
+      <c r="B57" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>198</v>
-      </c>
-      <c r="B49" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>199</v>
-      </c>
-      <c r="B50" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>202</v>
-      </c>
-      <c r="B51" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>205</v>
-      </c>
-      <c r="B52" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>206</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>208</v>
-      </c>
-      <c r="B54" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>211</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B58" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>213</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B59" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>215</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B60" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="B61" t="s">
         <v>217</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>218</v>
-      </c>
-      <c r="B59" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>56</v>
       </c>
-      <c r="B60" s="3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>57</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>58</v>
-      </c>
-      <c r="B62" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B62" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>59</v>
-      </c>
-      <c r="B63" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>62</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C64">
-        <v>4</v>
+        <v>224</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>184</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>185</v>
+        <v>57</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>84</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>85</v>
+        <v>58</v>
+      </c>
+      <c r="B66" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>86</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>87</v>
+        <v>59</v>
+      </c>
+      <c r="B67" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>93</v>
+        <v>63</v>
+      </c>
+      <c r="C68">
+        <v>4</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>75</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C69">
-        <v>2</v>
+        <v>183</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>76</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>136</v>
+        <v>84</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>122</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>123</v>
+        <v>75</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C73">
+        <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>94</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>95</v>
+        <v>76</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>98</v>
+        <v>122</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>100</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>98</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>102</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>104</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>117</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B84" s="4" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>106</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B85" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>108</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B86" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>110</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B87" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>111</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B88" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>119</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B89" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>112</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B90" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>113</v>
+      </c>
+      <c r="B91" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>114</v>
+      </c>
+      <c r="B92" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>115</v>
+      </c>
+      <c r="B93" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>113</v>
-      </c>
-      <c r="B87" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>114</v>
-      </c>
-      <c r="B88" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>115</v>
-      </c>
-      <c r="B89" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>125</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B94" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>127</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B95" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>128</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B96" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>116</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>131</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>132</v>
-      </c>
-      <c r="B95" t="s">
-        <v>133</v>
-      </c>
-      <c r="C95">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>138</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>140</v>
-      </c>
-      <c r="B97" t="s">
-        <v>139</v>
+        <v>116</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>141</v>
-      </c>
-      <c r="B98" t="s">
-        <v>162</v>
+        <v>131</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>142</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>143</v>
+        <v>132</v>
+      </c>
+      <c r="B99" t="s">
+        <v>133</v>
+      </c>
+      <c r="C99">
+        <v>3</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>144</v>
-      </c>
-      <c r="B100" t="s">
-        <v>174</v>
+        <v>138</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B101" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B102" t="s">
-        <v>147</v>
-      </c>
-      <c r="C102">
-        <v>3</v>
+        <v>162</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>149</v>
-      </c>
-      <c r="B103" t="s">
-        <v>150</v>
-      </c>
-      <c r="C103">
-        <v>3</v>
+        <v>142</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B104" t="s">
-        <v>152</v>
+        <v>174</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="B105" t="s">
-        <v>170</v>
-      </c>
-      <c r="C105">
-        <v>2</v>
+        <v>148</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="B106" t="s">
-        <v>191</v>
+        <v>147</v>
+      </c>
+      <c r="C106">
+        <v>3</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>175</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>192</v>
+        <v>149</v>
+      </c>
+      <c r="B107" t="s">
+        <v>150</v>
+      </c>
+      <c r="C107">
+        <v>3</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>176</v>
+        <v>151</v>
       </c>
       <c r="B108" t="s">
-        <v>194</v>
-      </c>
-      <c r="C108">
-        <v>2</v>
+        <v>152</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="B109" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="C109">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="B110" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>221</v>
-      </c>
-      <c r="B111" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B115" s="4"/>
-    </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B121" s="4"/>
-    </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B123" s="4"/>
-    </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B135" s="3"/>
-    </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B137" s="4"/>
-    </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B149" s="2"/>
+        <v>175</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>176</v>
+      </c>
+      <c r="B112" t="s">
+        <v>192</v>
+      </c>
+      <c r="C112">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>177</v>
+      </c>
+      <c r="B113" t="s">
+        <v>178</v>
+      </c>
+      <c r="C113">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>179</v>
+      </c>
+      <c r="B114" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>219</v>
+      </c>
+      <c r="B115" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B119" s="4"/>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B125" s="4"/>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B127" s="4"/>
+    </row>
+    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B139" s="3"/>
+    </row>
+    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B141" s="4"/>
     </row>
     <row r="153" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B153" s="2"/>
     </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B154" s="2"/>
-    </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B155" s="2"/>
-    </row>
     <row r="157" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B157" s="2"/>
     </row>
@@ -2034,9 +2081,6 @@
     <row r="159" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B159" s="2"/>
     </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B160" s="2"/>
-    </row>
     <row r="161" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B161" s="2"/>
     </row>
@@ -2046,14 +2090,26 @@
     <row r="163" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B163" s="2"/>
     </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B171" s="4"/>
-    </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B172" s="4"/>
-    </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B177" s="2"/>
+    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B164" s="2"/>
+    </row>
+    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B165" s="2"/>
+    </row>
+    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B166" s="2"/>
+    </row>
+    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B167" s="2"/>
+    </row>
+    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B175" s="4"/>
+    </row>
+    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B176" s="4"/>
+    </row>
+    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B181" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
refactor wheel motion explanation thing in act 2-1, using time slider instead
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F345774-E672-40BC-A0BB-739C22E558BC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FFD636-651F-4D0F-8596-E6A7F588112B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="235">
   <si>
     <t>Key</t>
   </si>
@@ -424,9 +424,6 @@
     <t>Targets Eliminated</t>
   </si>
   <si>
-    <t>The first few trails are where the knight was pushing the wheel. You can see that the distance between them are increasing.</t>
-  </si>
-  <si>
     <t>A vector is composed of a value for each axis. In this case, the x and y. These values can also tell us the direction, and the magnitude.</t>
   </si>
   <si>
@@ -580,12 +577,6 @@
     <t>A mighty knight has brought us a wheel to demonstrate. The wheel is enchanted with magical trails to allow us to observe its motion.</t>
   </si>
   <si>
-    <t>At this point, the distance between each trail is equal. This means that the net force acting on the wheel is zero.</t>
-  </si>
-  <si>
-    <t>The trails here are going down. We can observe that the only force acting on the wheel is gravity.</t>
-  </si>
-  <si>
     <t>The nefarious goblins have appeared out of thin air! They are surely up to no good. Push them off the cliff with the wheel.</t>
   </si>
   <si>
@@ -643,9 +634,6 @@
     <t>newton_first_law_dlg_goblins_1</t>
   </si>
   <si>
-    <t>The goblins are pushing back! This cancels out the knight's push.</t>
-  </si>
-  <si>
     <t>This means that an object will keep doing what it is doing, be it sitting or moving, until it is bothered by a bunch of forces (net force).</t>
   </si>
   <si>
@@ -713,6 +701,30 @@
   </si>
   <si>
     <t>The weight of an object is essentially the force of gravity.</t>
+  </si>
+  <si>
+    <t>secondsFormat</t>
+  </si>
+  <si>
+    <t>Drag the slider to observe the wheel's motion over time.</t>
+  </si>
+  <si>
+    <t>timeSliderWheelHint</t>
+  </si>
+  <si>
+    <t>The goblins are pushing back! This brings the net force (sum of forces) back to zero.</t>
+  </si>
+  <si>
+    <t>As the wheel falls, the velocity in the Y-axis starts to decrease.</t>
+  </si>
+  <si>
+    <t>The knight is pushing the wheel. The velocity in the X-axis is increasing.</t>
+  </si>
+  <si>
+    <t>The wheel continues to roll. There is no change in velocity.</t>
+  </si>
+  <si>
+    <t>{0:0.0} seconds</t>
   </si>
 </sst>
 </file>
@@ -1060,10 +1072,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D181"/>
+  <dimension ref="A1:D182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,7 +1119,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1206,34 +1218,34 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>164</v>
+      </c>
+      <c r="B15" t="s">
         <v>165</v>
-      </c>
-      <c r="B15" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>166</v>
+      </c>
+      <c r="B16" t="s">
         <v>167</v>
-      </c>
-      <c r="B16" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>162</v>
+      </c>
+      <c r="B17" t="s">
         <v>163</v>
-      </c>
-      <c r="B17" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>159</v>
+      </c>
+      <c r="B18" t="s">
         <v>160</v>
-      </c>
-      <c r="B18" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1268,7 +1280,7 @@
         <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C22">
         <v>3</v>
@@ -1276,10 +1288,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>153</v>
+      </c>
+      <c r="B23" t="s">
         <v>154</v>
-      </c>
-      <c r="B23" t="s">
-        <v>155</v>
       </c>
       <c r="C23">
         <v>1.5</v>
@@ -1287,10 +1299,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>155</v>
+      </c>
+      <c r="B24" t="s">
         <v>156</v>
-      </c>
-      <c r="B24" t="s">
-        <v>157</v>
       </c>
       <c r="C24">
         <v>1.5</v>
@@ -1298,10 +1310,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>157</v>
+      </c>
+      <c r="B25" t="s">
         <v>158</v>
-      </c>
-      <c r="B25" t="s">
-        <v>159</v>
       </c>
       <c r="C25">
         <v>1.5</v>
@@ -1371,7 +1383,7 @@
         <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1395,7 +1407,7 @@
         <v>51</v>
       </c>
       <c r="B36" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1424,10 +1436,10 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B40" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1472,510 +1484,507 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>72</v>
+        <v>227</v>
       </c>
       <c r="B46" t="s">
-        <v>124</v>
+        <v>234</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B47" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>225</v>
+        <v>64</v>
       </c>
       <c r="B48" t="s">
-        <v>226</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="B49" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>37</v>
+        <v>223</v>
       </c>
       <c r="B50" t="s">
-        <v>208</v>
+        <v>224</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>196</v>
+        <v>37</v>
       </c>
       <c r="B51" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B52" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B53" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B54" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>204</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
+      </c>
+      <c r="B55" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>206</v>
-      </c>
-      <c r="B56" t="s">
-        <v>207</v>
+        <v>201</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B57" t="s">
-        <v>210</v>
+        <v>230</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B58" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B59" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>215</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>218</v>
+        <v>209</v>
+      </c>
+      <c r="B60" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>216</v>
-      </c>
-      <c r="B61" t="s">
-        <v>217</v>
+        <v>211</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>56</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>222</v>
+        <v>212</v>
+      </c>
+      <c r="B62" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>223</v>
+        <v>56</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>57</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>181</v>
+        <v>220</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>58</v>
-      </c>
-      <c r="B66" t="s">
-        <v>182</v>
+        <v>57</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B67" t="s">
-        <v>221</v>
+        <v>181</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>62</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C68">
-        <v>4</v>
+        <v>59</v>
+      </c>
+      <c r="B68" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>183</v>
+        <v>62</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>184</v>
+        <v>63</v>
+      </c>
+      <c r="C69">
+        <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>84</v>
+        <v>182</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>85</v>
+        <v>183</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>75</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C73">
-        <v>2</v>
+        <v>88</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>76</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>136</v>
+        <v>75</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C74">
+        <v>2</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>89</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>92</v>
+        <v>76</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>122</v>
+        <v>90</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>123</v>
+        <v>91</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>94</v>
+        <v>122</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>106</v>
-      </c>
-      <c r="B85" t="s">
-        <v>107</v>
+        <v>117</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B86" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B87" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B88" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B89" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="B90" t="s">
-        <v>185</v>
+        <v>134</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B91" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B92" t="s">
-        <v>186</v>
+        <v>232</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B93" t="s">
-        <v>187</v>
+        <v>233</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B94" t="s">
-        <v>126</v>
+        <v>231</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B95" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B96" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>116</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>188</v>
+        <v>128</v>
+      </c>
+      <c r="B97" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>137</v>
+        <v>185</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>132</v>
-      </c>
-      <c r="B99" t="s">
-        <v>133</v>
-      </c>
-      <c r="C99">
-        <v>3</v>
+        <v>131</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>138</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>173</v>
+        <v>132</v>
+      </c>
+      <c r="B100" t="s">
+        <v>133</v>
+      </c>
+      <c r="C100">
+        <v>3</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>140</v>
-      </c>
-      <c r="B101" t="s">
-        <v>139</v>
+        <v>137</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B102" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>142</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
+      </c>
+      <c r="B103" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>144</v>
-      </c>
-      <c r="B104" t="s">
-        <v>174</v>
+        <v>141</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B105" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B106" t="s">
         <v>147</v>
       </c>
-      <c r="C106">
-        <v>3</v>
-      </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B107" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C107">
         <v>3</v>
@@ -1983,97 +1992,113 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B108" t="s">
-        <v>152</v>
+        <v>149</v>
+      </c>
+      <c r="C108">
+        <v>3</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="B109" t="s">
-        <v>170</v>
-      </c>
-      <c r="C109">
-        <v>2</v>
+        <v>151</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B110" t="s">
-        <v>189</v>
+        <v>169</v>
+      </c>
+      <c r="C110">
+        <v>2</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>175</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>190</v>
+        <v>171</v>
+      </c>
+      <c r="B111" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>176</v>
-      </c>
-      <c r="B112" t="s">
-        <v>192</v>
-      </c>
-      <c r="C112">
-        <v>2</v>
+        <v>174</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B113" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="C113">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B114" t="s">
-        <v>180</v>
+        <v>177</v>
+      </c>
+      <c r="C114">
+        <v>3</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>219</v>
+        <v>178</v>
       </c>
       <c r="B115" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B119" s="4"/>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B125" s="4"/>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B127" s="4"/>
-    </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B139" s="3"/>
-    </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B141" s="4"/>
-    </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B153" s="2"/>
-    </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B157" s="2"/>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>215</v>
+      </c>
+      <c r="B116" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>229</v>
+      </c>
+      <c r="B117" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B120" s="4"/>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B126" s="4"/>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B128" s="4"/>
+    </row>
+    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B140" s="3"/>
+    </row>
+    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B142" s="4"/>
+    </row>
+    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B154" s="2"/>
     </row>
     <row r="158" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B158" s="2"/>
@@ -2081,8 +2106,8 @@
     <row r="159" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B159" s="2"/>
     </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B161" s="2"/>
+    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B160" s="2"/>
     </row>
     <row r="162" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B162" s="2"/>
@@ -2102,14 +2127,17 @@
     <row r="167" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B167" s="2"/>
     </row>
-    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B175" s="4"/>
+    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B168" s="2"/>
     </row>
     <row r="176" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B176" s="4"/>
     </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B181" s="2"/>
+    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B177" s="4"/>
+    </row>
+    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B182" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
revamp act 2-1 illustrations
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FFD636-651F-4D0F-8596-E6A7F588112B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076AB7D1-E42A-4C3D-A012-1E97B48DCAD8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="239">
   <si>
     <t>Key</t>
   </si>
@@ -424,9 +424,6 @@
     <t>Targets Eliminated</t>
   </si>
   <si>
-    <t>A vector is composed of a value for each axis. In this case, the x and y. These values can also tell us the direction, and the magnitude.</t>
-  </si>
-  <si>
     <t>Newton's second law states that the acceleration of an object is proportional to the net force acting on it, and inversely proportional to its mass.</t>
   </si>
   <si>
@@ -725,6 +722,21 @@
   </si>
   <si>
     <t>{0:0.0} seconds</t>
+  </si>
+  <si>
+    <t>knightsForcePush</t>
+  </si>
+  <si>
+    <t>Knight's Force Push</t>
+  </si>
+  <si>
+    <t>A vector has a value for each axis. In this case, the x and y. These values can tell us the direction, and the magnitude.</t>
+  </si>
+  <si>
+    <t>wheelsAcceleration</t>
+  </si>
+  <si>
+    <t>Wheel's Acceleration</t>
   </si>
 </sst>
 </file>
@@ -1074,8 +1086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1119,7 +1131,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1218,34 +1230,34 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>163</v>
+      </c>
+      <c r="B15" t="s">
         <v>164</v>
-      </c>
-      <c r="B15" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B16" t="s">
         <v>166</v>
-      </c>
-      <c r="B16" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>161</v>
+      </c>
+      <c r="B17" t="s">
         <v>162</v>
-      </c>
-      <c r="B17" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>158</v>
+      </c>
+      <c r="B18" t="s">
         <v>159</v>
-      </c>
-      <c r="B18" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1280,7 +1292,7 @@
         <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C22">
         <v>3</v>
@@ -1288,10 +1300,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>152</v>
+      </c>
+      <c r="B23" t="s">
         <v>153</v>
-      </c>
-      <c r="B23" t="s">
-        <v>154</v>
       </c>
       <c r="C23">
         <v>1.5</v>
@@ -1299,10 +1311,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>154</v>
+      </c>
+      <c r="B24" t="s">
         <v>155</v>
-      </c>
-      <c r="B24" t="s">
-        <v>156</v>
       </c>
       <c r="C24">
         <v>1.5</v>
@@ -1310,10 +1322,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>156</v>
+      </c>
+      <c r="B25" t="s">
         <v>157</v>
-      </c>
-      <c r="B25" t="s">
-        <v>158</v>
       </c>
       <c r="C25">
         <v>1.5</v>
@@ -1383,7 +1395,7 @@
         <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1407,7 +1419,7 @@
         <v>51</v>
       </c>
       <c r="B36" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1436,10 +1448,10 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>189</v>
+      </c>
+      <c r="B40" t="s">
         <v>190</v>
-      </c>
-      <c r="B40" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1484,10 +1496,10 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1508,18 +1520,18 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>220</v>
+      </c>
+      <c r="B49" t="s">
         <v>221</v>
-      </c>
-      <c r="B49" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>222</v>
+      </c>
+      <c r="B50" t="s">
         <v>223</v>
-      </c>
-      <c r="B50" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1527,95 +1539,95 @@
         <v>37</v>
       </c>
       <c r="B51" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B52" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B53" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>196</v>
+      </c>
+      <c r="B54" t="s">
         <v>197</v>
-      </c>
-      <c r="B54" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B55" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>200</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>201</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B57" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>204</v>
+      </c>
+      <c r="B58" t="s">
         <v>205</v>
-      </c>
-      <c r="B58" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>206</v>
+      </c>
+      <c r="B59" t="s">
         <v>207</v>
-      </c>
-      <c r="B59" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>208</v>
+      </c>
+      <c r="B60" t="s">
         <v>209</v>
-      </c>
-      <c r="B60" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>211</v>
+      </c>
+      <c r="B62" t="s">
         <v>212</v>
-      </c>
-      <c r="B62" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1623,23 +1635,23 @@
         <v>56</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1647,7 +1659,7 @@
         <v>57</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1655,7 +1667,7 @@
         <v>58</v>
       </c>
       <c r="B67" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1663,7 +1675,7 @@
         <v>59</v>
       </c>
       <c r="B68" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1679,10 +1691,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>181</v>
+      </c>
+      <c r="B70" s="4" t="s">
         <v>182</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -1725,7 +1737,7 @@
         <v>76</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -1845,7 +1857,7 @@
         <v>119</v>
       </c>
       <c r="B90" t="s">
-        <v>134</v>
+        <v>236</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -1853,7 +1865,7 @@
         <v>112</v>
       </c>
       <c r="B91" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -1861,7 +1873,7 @@
         <v>113</v>
       </c>
       <c r="B92" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -1869,7 +1881,7 @@
         <v>114</v>
       </c>
       <c r="B93" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -1877,7 +1889,7 @@
         <v>115</v>
       </c>
       <c r="B94" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -1909,7 +1921,7 @@
         <v>116</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -1917,7 +1929,7 @@
         <v>131</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -1933,58 +1945,58 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B102" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B103" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
+        <v>140</v>
+      </c>
+      <c r="B104" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B105" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B106" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
+        <v>144</v>
+      </c>
+      <c r="B107" t="s">
         <v>145</v>
-      </c>
-      <c r="B107" t="s">
-        <v>146</v>
       </c>
       <c r="C107">
         <v>3</v>
@@ -1992,10 +2004,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
+        <v>147</v>
+      </c>
+      <c r="B108" t="s">
         <v>148</v>
-      </c>
-      <c r="B108" t="s">
-        <v>149</v>
       </c>
       <c r="C108">
         <v>3</v>
@@ -2003,18 +2015,18 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
+        <v>149</v>
+      </c>
+      <c r="B109" t="s">
         <v>150</v>
-      </c>
-      <c r="B109" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
+        <v>167</v>
+      </c>
+      <c r="B110" t="s">
         <v>168</v>
-      </c>
-      <c r="B110" t="s">
-        <v>169</v>
       </c>
       <c r="C110">
         <v>2</v>
@@ -2022,26 +2034,26 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B111" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B113" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C113">
         <v>2</v>
@@ -2049,10 +2061,10 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
+        <v>175</v>
+      </c>
+      <c r="B114" t="s">
         <v>176</v>
-      </c>
-      <c r="B114" t="s">
-        <v>177</v>
       </c>
       <c r="C114">
         <v>3</v>
@@ -2060,26 +2072,42 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
+        <v>177</v>
+      </c>
+      <c r="B115" t="s">
         <v>178</v>
-      </c>
-      <c r="B115" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
+        <v>214</v>
+      </c>
+      <c r="B116" t="s">
         <v>215</v>
-      </c>
-      <c r="B116" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B117" t="s">
-        <v>228</v>
+        <v>227</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>234</v>
+      </c>
+      <c r="B118" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>237</v>
+      </c>
+      <c r="B119" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
some more tweaks, updated build
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4A95EB-FE29-4D2B-8EF0-4151CDA540A3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59AE57F-2D91-4C36-9C67-AC8A730E214A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -532,9 +532,6 @@
     <t>Drag this to adjust the cannon's angle.</t>
   </si>
   <si>
-    <t>As you fire away, observe that the projectile will move at a constant velocity along the X-axis.</t>
-  </si>
-  <si>
     <t>act_2_end_dlg_2</t>
   </si>
   <si>
@@ -652,15 +649,9 @@
     <t>We have enough knights to overcome this force. Summon the mighty knights for this one last push!</t>
   </si>
   <si>
-    <t>This block has no wheels. The force of friction will allow the block to resist a certain amount of push or pull from all sides.</t>
-  </si>
-  <si>
     <t>hintTooltip</t>
   </si>
   <si>
-    <t>Here's a locked treasure chest as a demonstration. Put the correct amount of weight on the other platform to unlock it.</t>
-  </si>
-  <si>
     <t>In this scenario, we will learn more about inertia.</t>
   </si>
   <si>
@@ -685,9 +676,6 @@
     <t>Mass is a measure of inertia. It tells us how much resistance an object has in changing motion.</t>
   </si>
   <si>
-    <t>The weight of an object is essentially the force of gravity.</t>
-  </si>
-  <si>
     <t>secondsFormat</t>
   </si>
   <si>
@@ -737,6 +725,18 @@
   </si>
   <si>
     <t>Press this button to show hints. You can press it again later to show more.</t>
+  </si>
+  <si>
+    <t>This block has no wheels. The force of friction will allow the block to resist a certain amount of push or pull from the sides.</t>
+  </si>
+  <si>
+    <t>The weight of an object is essentially the force of gravity. The more mass an object has, the heavier it gets.</t>
+  </si>
+  <si>
+    <t>Here's a locked treasure chest as a demonstration. Put the correct amount of weight on the other platform to unlock it!</t>
+  </si>
+  <si>
+    <t>The cannon can launch projectiles at different directions by adjusting its angle. This will allow us to hit targets at various heights.</t>
   </si>
 </sst>
 </file>
@@ -1086,8 +1086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="B116" sqref="B116"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1395,7 +1395,7 @@
         <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1419,7 +1419,7 @@
         <v>51</v>
       </c>
       <c r="B36" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1448,10 +1448,10 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>185</v>
+      </c>
+      <c r="B40" t="s">
         <v>186</v>
-      </c>
-      <c r="B40" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1496,10 +1496,10 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B46" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1520,18 +1520,18 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B49" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B50" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1539,95 +1539,95 @@
         <v>37</v>
       </c>
       <c r="B51" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B52" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B53" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>192</v>
+      </c>
+      <c r="B54" t="s">
         <v>193</v>
-      </c>
-      <c r="B54" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B55" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>196</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B57" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>200</v>
+      </c>
+      <c r="B58" t="s">
         <v>201</v>
-      </c>
-      <c r="B58" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>202</v>
+      </c>
+      <c r="B59" t="s">
         <v>203</v>
-      </c>
-      <c r="B59" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>204</v>
+      </c>
+      <c r="B60" t="s">
         <v>205</v>
-      </c>
-      <c r="B60" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>210</v>
+        <v>235</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>207</v>
+      </c>
+      <c r="B62" t="s">
         <v>208</v>
-      </c>
-      <c r="B62" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1635,23 +1635,23 @@
         <v>56</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>221</v>
+        <v>236</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1659,7 +1659,7 @@
         <v>57</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1667,7 +1667,7 @@
         <v>58</v>
       </c>
       <c r="B67" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1675,7 +1675,7 @@
         <v>59</v>
       </c>
       <c r="B68" t="s">
-        <v>212</v>
+        <v>237</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1691,10 +1691,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>178</v>
+      </c>
+      <c r="B70" s="4" t="s">
         <v>179</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -1849,7 +1849,7 @@
         <v>117</v>
       </c>
       <c r="B89" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -1857,7 +1857,7 @@
         <v>110</v>
       </c>
       <c r="B90" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -1865,7 +1865,7 @@
         <v>111</v>
       </c>
       <c r="B91" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -1873,7 +1873,7 @@
         <v>112</v>
       </c>
       <c r="B92" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -1881,7 +1881,7 @@
         <v>113</v>
       </c>
       <c r="B93" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -1913,7 +1913,7 @@
         <v>114</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -1972,7 +1972,7 @@
         <v>140</v>
       </c>
       <c r="B104" t="s">
-        <v>170</v>
+        <v>238</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -2029,31 +2029,31 @@
         <v>168</v>
       </c>
       <c r="B110" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B113" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C113">
         <v>2</v>
@@ -2061,10 +2061,10 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
+        <v>172</v>
+      </c>
+      <c r="B114" t="s">
         <v>173</v>
-      </c>
-      <c r="B114" t="s">
-        <v>174</v>
       </c>
       <c r="C114">
         <v>3</v>
@@ -2072,42 +2072,42 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
+        <v>174</v>
+      </c>
+      <c r="B115" t="s">
         <v>175</v>
-      </c>
-      <c r="B115" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B116" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B117" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B118" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B119" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
info change on inertia in act 1-2 added drag instruct visual in act 1-2 slightly lower default volumes
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59AE57F-2D91-4C36-9C67-AC8A730E214A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E20B140-94A8-4B00-B220-002389E9581B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="3120" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -664,18 +664,12 @@
     <t>mass_inertia</t>
   </si>
   <si>
-    <t>Mass = Inertia</t>
-  </si>
-  <si>
     <t>weight_gravity</t>
   </si>
   <si>
     <t>Weight = Force of Gravity</t>
   </si>
   <si>
-    <t>Mass is a measure of inertia. It tells us how much resistance an object has in changing motion.</t>
-  </si>
-  <si>
     <t>secondsFormat</t>
   </si>
   <si>
@@ -730,13 +724,19 @@
     <t>This block has no wheels. The force of friction will allow the block to resist a certain amount of push or pull from the sides.</t>
   </si>
   <si>
-    <t>The weight of an object is essentially the force of gravity. The more mass an object has, the heavier it gets.</t>
-  </si>
-  <si>
     <t>Here's a locked treasure chest as a demonstration. Put the correct amount of weight on the other platform to unlock it!</t>
   </si>
   <si>
     <t>The cannon can launch projectiles at different directions by adjusting its angle. This will allow us to hit targets at various heights.</t>
+  </si>
+  <si>
+    <t>Inertia is proportional to Mass</t>
+  </si>
+  <si>
+    <t>Inertia tells us how much resistance an object has in changing motion. It is proportional to the amount of mass of the object.</t>
+  </si>
+  <si>
+    <t>Mass measures the amount of matter the object contains. The more mass an object has, the heavier it gets, and more harder to move.</t>
   </si>
 </sst>
 </file>
@@ -1086,8 +1086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B110" sqref="B110"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1496,10 +1496,10 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B46" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1523,15 +1523,15 @@
         <v>213</v>
       </c>
       <c r="B49" t="s">
-        <v>214</v>
+        <v>236</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>214</v>
+      </c>
+      <c r="B50" t="s">
         <v>215</v>
-      </c>
-      <c r="B50" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1587,7 +1587,7 @@
         <v>198</v>
       </c>
       <c r="B57" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1619,7 +1619,7 @@
         <v>206</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -1643,7 +1643,7 @@
         <v>211</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1651,7 +1651,7 @@
         <v>212</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1675,7 +1675,7 @@
         <v>59</v>
       </c>
       <c r="B68" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1849,7 +1849,7 @@
         <v>117</v>
       </c>
       <c r="B89" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -1865,7 +1865,7 @@
         <v>111</v>
       </c>
       <c r="B91" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -1873,7 +1873,7 @@
         <v>112</v>
       </c>
       <c r="B92" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -1881,7 +1881,7 @@
         <v>113</v>
       </c>
       <c r="B93" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -1972,7 +1972,7 @@
         <v>140</v>
       </c>
       <c r="B104" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -2029,7 +2029,7 @@
         <v>168</v>
       </c>
       <c r="B110" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -2042,10 +2042,10 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -2083,31 +2083,31 @@
         <v>209</v>
       </c>
       <c r="B116" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B117" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B118" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B119" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added spanish translations, some fix to spanish typos
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E20B140-94A8-4B00-B220-002389E9581B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59A8E4D-20BA-429E-B6AE-0269E6151E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="3120" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2775" yWindow="2505" windowWidth="22875" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
+    <sheet name="es" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="354">
   <si>
     <t>Key</t>
   </si>
@@ -737,6 +738,351 @@
   </si>
   <si>
     <t>Mass measures the amount of matter the object contains. The more mass an object has, the heavier it gets, and more harder to move.</t>
+  </si>
+  <si>
+    <t>¡Bienvenido!</t>
+  </si>
+  <si>
+    <t>¡Los duendes están empujando hacia atrás! Esto hace que la fuerza neta (suma de fuerzas) vuelva a cero.</t>
+  </si>
+  <si>
+    <t>Caballeros poderosos de la fuerza\n&lt;size=30&gt;Ley 1 y 2 de Newton&lt;/size&gt;</t>
+  </si>
+  <si>
+    <t>OPCIONES</t>
+  </si>
+  <si>
+    <t>MÚSICA</t>
+  </si>
+  <si>
+    <t>SONIDO</t>
+  </si>
+  <si>
+    <t>APAGADO</t>
+  </si>
+  <si>
+    <t>ENCENDIDO</t>
+  </si>
+  <si>
+    <t>CERRAR</t>
+  </si>
+  <si>
+    <t>SÍ</t>
+  </si>
+  <si>
+    <t>¿Estás seguro de que quieres reiniciar el nivel?</t>
+  </si>
+  <si>
+    <t>REINICIAR</t>
+  </si>
+  <si>
+    <t>CRÉDITOS</t>
+  </si>
+  <si>
+    <t>Escrito por: David Dionisio\r\nMúsica de: Kevin MacLeod</t>
+  </si>
+  <si>
+    <t>COMENZAR</t>
+  </si>
+  <si>
+    <t>PROCEDER</t>
+  </si>
+  <si>
+    <t>VICTORIA</t>
+  </si>
+  <si>
+    <t>velocidad (x)</t>
+  </si>
+  <si>
+    <t>velocidad (y)</t>
+  </si>
+  <si>
+    <t>¡La princesa ha sido rescatada!</t>
+  </si>
+  <si>
+    <t>Acto 1</t>
+  </si>
+  <si>
+    <t>Acto 2</t>
+  </si>
+  <si>
+    <t>Acto 3</t>
+  </si>
+  <si>
+    <t>Primera ley de Newton</t>
+  </si>
+  <si>
+    <t>La primera ley de Newton establece que un objeto en reposo permanecerá en reposo y que un objeto en movimiento mantendrá una velocidad constante a menos que actúe una fuerza externa neta.</t>
+  </si>
+  <si>
+    <t>En reposo</t>
+  </si>
+  <si>
+    <t>En movimiento</t>
+  </si>
+  <si>
+    <t>Fuerza equilibrada.</t>
+  </si>
+  <si>
+    <t>Aceleración = 0 m/s²</t>
+  </si>
+  <si>
+    <t>Gravedad de fuerza</t>
+  </si>
+  <si>
+    <t>Tierra de fuerza</t>
+  </si>
+  <si>
+    <t>Fuerza fricción</t>
+  </si>
+  <si>
+    <t>Fuerza empuje</t>
+  </si>
+  <si>
+    <t>0 Fuerza neta (balanceada)</t>
+  </si>
+  <si>
+    <t>Fuerza</t>
+  </si>
+  <si>
+    <t>Fuerza equilibrada</t>
+  </si>
+  <si>
+    <t>Fuerza desequilibrada</t>
+  </si>
+  <si>
+    <t>Fuerza neta</t>
+  </si>
+  <si>
+    <t>Peso</t>
+  </si>
+  <si>
+    <t>POSICIÓN</t>
+  </si>
+  <si>
+    <t>VELOCIDAD</t>
+  </si>
+  <si>
+    <t>ACELERACIÓN</t>
+  </si>
+  <si>
+    <t>Eje</t>
+  </si>
+  <si>
+    <t>{0:0.0} segundos</t>
+  </si>
+  <si>
+    <t>Tiempo: {0:0.0} - {1:0.0} segundos</t>
+  </si>
+  <si>
+    <t>LANZAMIENTO</t>
+  </si>
+  <si>
+    <t>La inercia es proporcional a la masa</t>
+  </si>
+  <si>
+    <t>Peso = Fuerza de gravedad</t>
+  </si>
+  <si>
+    <t>Esto significa que un objeto seguirá haciendo lo mismo, ya sea sentado o en movimiento, hasta que le molestan un montón de fuerzas (fuerza neta).</t>
+  </si>
+  <si>
+    <t>¡Oh, no! ¡La princesa ha sido tomada como rehén por estos nefastos duendes!</t>
+  </si>
+  <si>
+    <t>Permítanme dejar caer un objeto que nos ayudará en esta situación. Esto nos mostrará la primera ley en acción.</t>
+  </si>
+  <si>
+    <t>La fuerza de gravedad está tirando del objeto hacia la Tierra, lo que le permite caer.</t>
+  </si>
+  <si>
+    <t>Ahora que el objeto ha aterrizado, el suelo lo empuja hacia arriba. Esto cancela la fuerza de gravedad. El objeto está en reposo.</t>
+  </si>
+  <si>
+    <t>¡Adelante y llama a un caballero poderoso para empujar el objeto!</t>
+  </si>
+  <si>
+    <t>¡Invoca a más caballeros para vencer a los duendes del otro lado!</t>
+  </si>
+  <si>
+    <t>¡Excelente! Como puede ver, el lado con más fuerza determinará la dirección de la fuerza neta que actúa sobre el objeto.</t>
+  </si>
+  <si>
+    <t>¡Necesitamos un bloque más para rescatar a nuestra damisela en apuros!</t>
+  </si>
+  <si>
+    <t>Este bloque no tiene ruedas. La fuerza de fricción permitirá que el bloque resista una cierta cantidad de empuje o tirón de los lados.</t>
+  </si>
+  <si>
+    <t>Tenemos suficientes caballeros para superar esta fuerza. ¡Invoca a los poderosos caballeros para este último empujón!</t>
+  </si>
+  <si>
+    <t>En este escenario, aprenderemos más sobre la inercia.</t>
+  </si>
+  <si>
+    <t>La inercia nos indica cuánta resistencia tiene un objeto al cambiar de movimiento. Es proporcional a la cantidad de masa del objeto.</t>
+  </si>
+  <si>
+    <t>La masa mide la cantidad de materia que contiene el objeto. Cuanto más masa tiene un objeto, más pesado se vuelve y más difícil de mover.</t>
+  </si>
+  <si>
+    <t>Observe cómo interactúan las fuerzas en esta escala de balance.</t>
+  </si>
+  <si>
+    <t>El peso de cada plataforma hace que la báscula se incline. Si ambas plataformas tienen el mismo peso, se alinearán horizontalmente.</t>
+  </si>
+  <si>
+    <t>Aquí hay un cofre del tesoro cerrado como demostración. Pon la cantidad correcta de peso en la otra plataforma para desbloquearla.</t>
+  </si>
+  <si>
+    <t>¡Has abierto el cofre del tesoro! He aquí, las riquezas descubiertas:</t>
+  </si>
+  <si>
+    <t>Arrastre estos pesos por encima de la plataforma.</t>
+  </si>
+  <si>
+    <t>Caballero empujando</t>
+  </si>
+  <si>
+    <t>Movimiento constante</t>
+  </si>
+  <si>
+    <t>Caída debido a la gravedad</t>
+  </si>
+  <si>
+    <t>Segunda ley de Newton</t>
+  </si>
+  <si>
+    <t>La segunda ley de Newton establece que la aceleración de un objeto es proporcional a la fuerza neta que actúa sobre él e inversamente proporcional a su masa.</t>
+  </si>
+  <si>
+    <t>Pulse el botón LANZAMIENTO.</t>
+  </si>
+  <si>
+    <t>Pulse el botón GRÁFICO.</t>
+  </si>
+  <si>
+    <t>Arrastre el control deslizante para cambiar el valor De la fuersa.</t>
+  </si>
+  <si>
+    <t>Masa</t>
+  </si>
+  <si>
+    <t>Aceleración</t>
+  </si>
+  <si>
+    <t>Velocidad</t>
+  </si>
+  <si>
+    <t>Dirección</t>
+  </si>
+  <si>
+    <t>Magnitud</t>
+  </si>
+  <si>
+    <t>Ejemplos</t>
+  </si>
+  <si>
+    <t>La aceleración es lo que hace que la velocidad de un objeto cambie con el tiempo. Lo que significa que el objeto acelerará, ralentizará o cambiará de dirección.</t>
+  </si>
+  <si>
+    <t>Como puedes ver, cuanta más masa tenga un objeto, menos acelerará desde la fuerza neta.</t>
+  </si>
+  <si>
+    <t>Tenga en cuenta que: fuerza, aceleración y velocidad son vectores.</t>
+  </si>
+  <si>
+    <t>Un vector tiene un valor para cada eje. En este caso, las x e y. Estos valores pueden indicarnos la dirección y la magnitud.</t>
+  </si>
+  <si>
+    <t>Un caballero poderoso nos ha traído una rueda para demostrarnos. La rueda está encantada con senderos mágicos para permitirnos observar su movimiento.</t>
+  </si>
+  <si>
+    <t>El caballero empuja el volante. La velocidad en el eje X está aumentando.</t>
+  </si>
+  <si>
+    <t>La rueda sigue rodando. No hay cambios en la velocidad.</t>
+  </si>
+  <si>
+    <t>A medida que cae la rueda, la velocidad en el eje Y comienza a disminuir.</t>
+  </si>
+  <si>
+    <t>El gráfico asigna los senderos a lo largo del tiempo a lo largo de los ejes x e y. Asegúrese de comprobar la velocidad y la aceleración desplazándose hacia abajo.</t>
+  </si>
+  <si>
+    <t>Observe cómo se curva la línea de posición a medida que aumenta la velocidad, lo que indica que hay aceleración.</t>
+  </si>
+  <si>
+    <t>Si la línea de posición es recta, la velocidad es constante y, por lo tanto, no hay aceleración.</t>
+  </si>
+  <si>
+    <t>¡Los nefastos duendes han aparecido de la nada! Seguramente no están tramando nada bueno. Empújalos por el acantilado con el volante.</t>
+  </si>
+  <si>
+    <t>Pulsa este botón cuando estés listo para continuar.</t>
+  </si>
+  <si>
+    <t>Objetivos eliminados</t>
+  </si>
+  <si>
+    <t>Arrastra esto para guiar el ángulo del cañón.</t>
+  </si>
+  <si>
+    <t>Recuerda revisar el gráfico para analizar la trayectoria de la bala de cañón.</t>
+  </si>
+  <si>
+    <t>¡Cuidado! ¡Han aparecido más duendes!</t>
+  </si>
+  <si>
+    <t>¡Vamos a sacar el poderoso cañón para vencer a estas alimañas!</t>
+  </si>
+  <si>
+    <t>El cañón puede lanzar proyectiles en diferentes direcciones ajustando su ángulo. Esto nos permitirá alcanzar objetivos a distintas alturas.</t>
+  </si>
+  <si>
+    <t>Arrastre el campo de fuerza a esta superficie.</t>
+  </si>
+  <si>
+    <t>Puede cambiar la posición de un campo de fuerza arrastrándolo.</t>
+  </si>
+  <si>
+    <t>Pulsa este botón para iniciar la simulación.</t>
+  </si>
+  <si>
+    <t>Mantén pulsado el botón de la papelera para borrar los campos de fuerza.</t>
+  </si>
+  <si>
+    <t>El Balón de Oro</t>
+  </si>
+  <si>
+    <t>¡Un gran meteorito se acerca a la Tierra! ¡La destrucción total nos espera si no se hace nada!</t>
+  </si>
+  <si>
+    <t>Busca la bola de oro, porque te dará la fuerza para frustrar la inminente fatalidad.</t>
+  </si>
+  <si>
+    <t>Con su conocimiento de la ley del movimiento de Newton, estoy seguro de que puede cumplir la tarea.</t>
+  </si>
+  <si>
+    <t>LA GLORIA ES TUYA</t>
+  </si>
+  <si>
+    <t>¡Gracias por jugar!</t>
+  </si>
+  <si>
+    <t>FINALIZAR</t>
+  </si>
+  <si>
+    <t>Pulsa este botón para mostrar sugerencias. Puedes volver a presionarlo más tarde para mostrar más.</t>
+  </si>
+  <si>
+    <t>Arrastre el control deslizante para observar el movimiento de la rueda a lo largo del tiempo.</t>
+  </si>
+  <si>
+    <t>Empuje de fuerza del caballero</t>
+  </si>
+  <si>
+    <t>Aceleración de la rueda</t>
   </si>
 </sst>
 </file>
@@ -793,7 +1139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -803,7 +1149,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1084,10 +1429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D182"/>
+  <dimension ref="A1:D119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1736,7 +2081,7 @@
       <c r="A75" t="s">
         <v>76</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2109,66 +2454,1042 @@
       <c r="B119" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B120" s="4"/>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B126" s="4"/>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B128" s="4"/>
-    </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B140" s="3"/>
-    </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B142" s="4"/>
-    </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B154" s="2"/>
-    </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B158" s="2"/>
-    </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B159" s="2"/>
-    </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B160" s="2"/>
-    </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B162" s="2"/>
-    </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B163" s="2"/>
-    </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B164" s="2"/>
-    </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B165" s="2"/>
-    </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B166" s="2"/>
-    </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B167" s="2"/>
-    </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B168" s="2"/>
-    </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B176" s="4"/>
-    </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B177" s="4"/>
-    </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B182" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A083F05-0FAA-4E78-9E79-0348AF6ADFB8}">
+  <dimension ref="A1:D119"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.28515625" customWidth="1"/>
+    <col min="2" max="2" width="87.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C2">
+        <v>1.5</v>
+      </c>
+      <c r="D2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>249</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>250</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B15" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>163</v>
+      </c>
+      <c r="B16" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>159</v>
+      </c>
+      <c r="B17" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>156</v>
+      </c>
+      <c r="B18" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" t="s">
+        <v>255</v>
+      </c>
+      <c r="C19">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s">
+        <v>258</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>150</v>
+      </c>
+      <c r="B23" t="s">
+        <v>259</v>
+      </c>
+      <c r="C23">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>152</v>
+      </c>
+      <c r="B24" t="s">
+        <v>260</v>
+      </c>
+      <c r="C24">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>154</v>
+      </c>
+      <c r="B25" t="s">
+        <v>261</v>
+      </c>
+      <c r="C25">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>79</v>
+      </c>
+      <c r="B37" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>82</v>
+      </c>
+      <c r="B39" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>185</v>
+      </c>
+      <c r="B40" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>66</v>
+      </c>
+      <c r="B42" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>67</v>
+      </c>
+      <c r="B43" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>73</v>
+      </c>
+      <c r="B45" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>216</v>
+      </c>
+      <c r="B46" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>64</v>
+      </c>
+      <c r="B48" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>213</v>
+      </c>
+      <c r="B49" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>214</v>
+      </c>
+      <c r="B50" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>37</v>
+      </c>
+      <c r="B51" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>188</v>
+      </c>
+      <c r="B52" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>189</v>
+      </c>
+      <c r="B53" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>192</v>
+      </c>
+      <c r="B54" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>195</v>
+      </c>
+      <c r="B55" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>196</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>198</v>
+      </c>
+      <c r="B57" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>200</v>
+      </c>
+      <c r="B58" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>202</v>
+      </c>
+      <c r="B59" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>204</v>
+      </c>
+      <c r="B60" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>206</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>207</v>
+      </c>
+      <c r="B62" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>56</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>211</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>212</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>57</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>58</v>
+      </c>
+      <c r="B67" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>59</v>
+      </c>
+      <c r="B68" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>62</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="C69">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>178</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>84</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>86</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>88</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>75</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>76</v>
+      </c>
+      <c r="B75" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>89</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>90</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>120</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>94</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>96</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>100</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>98</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>102</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>104</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>115</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>106</v>
+      </c>
+      <c r="B86" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>108</v>
+      </c>
+      <c r="B87" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>109</v>
+      </c>
+      <c r="B88" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>117</v>
+      </c>
+      <c r="B89" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>110</v>
+      </c>
+      <c r="B90" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>111</v>
+      </c>
+      <c r="B91" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>112</v>
+      </c>
+      <c r="B92" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>113</v>
+      </c>
+      <c r="B93" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>123</v>
+      </c>
+      <c r="B94" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>125</v>
+      </c>
+      <c r="B95" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>126</v>
+      </c>
+      <c r="B96" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>114</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>129</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>130</v>
+      </c>
+      <c r="B99" t="s">
+        <v>333</v>
+      </c>
+      <c r="C99">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>134</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>136</v>
+      </c>
+      <c r="B101" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>137</v>
+      </c>
+      <c r="B102" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>138</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>140</v>
+      </c>
+      <c r="B104" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>141</v>
+      </c>
+      <c r="B105" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>142</v>
+      </c>
+      <c r="B106" t="s">
+        <v>340</v>
+      </c>
+      <c r="C106">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>145</v>
+      </c>
+      <c r="B107" t="s">
+        <v>341</v>
+      </c>
+      <c r="C107">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>147</v>
+      </c>
+      <c r="B108" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>165</v>
+      </c>
+      <c r="B109" t="s">
+        <v>343</v>
+      </c>
+      <c r="C109">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>168</v>
+      </c>
+      <c r="B110" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>170</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>230</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>171</v>
+      </c>
+      <c r="B113" t="s">
+        <v>347</v>
+      </c>
+      <c r="C113">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>172</v>
+      </c>
+      <c r="B114" t="s">
+        <v>348</v>
+      </c>
+      <c r="C114">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>174</v>
+      </c>
+      <c r="B115" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>209</v>
+      </c>
+      <c r="B116" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>218</v>
+      </c>
+      <c r="B117" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>224</v>
+      </c>
+      <c r="B118" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>227</v>
+      </c>
+      <c r="B119" t="s">
+        <v>353</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
refactor options: changed volumes to sliders, added toggle speech
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59A8E4D-20BA-429E-B6AE-0269E6151E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D4AA64-62A2-4656-A3B0-2BB5D7B8945E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2775" yWindow="2505" windowWidth="22875" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5460" yWindow="3870" windowWidth="22875" windowHeight="15420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="357">
   <si>
     <t>Key</t>
   </si>
@@ -1083,6 +1083,15 @@
   </si>
   <si>
     <t>Aceleración de la rueda</t>
+  </si>
+  <si>
+    <t>speech</t>
+  </si>
+  <si>
+    <t>SPEECH</t>
+  </si>
+  <si>
+    <t>DISCURSO</t>
   </si>
 </sst>
 </file>
@@ -1429,10 +1438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D119"/>
+  <dimension ref="A1:D120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2455,6 +2464,14 @@
         <v>228</v>
       </c>
     </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>354</v>
+      </c>
+      <c r="B120" t="s">
+        <v>355</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2463,10 +2480,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A083F05-0FAA-4E78-9E79-0348AF6ADFB8}">
-  <dimension ref="A1:D119"/>
+  <dimension ref="A1:D120"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3489,6 +3506,14 @@
         <v>353</v>
       </c>
     </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>354</v>
+      </c>
+      <c r="B120" t="s">
+        <v>356</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
auto-complete game at end, remove act 3-5
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D4AA64-62A2-4656-A3B0-2BB5D7B8945E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0151F04C-C9C9-497E-A3F0-5FEA3E70A6BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5460" yWindow="3870" windowWidth="22875" windowHeight="15420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5460" yWindow="3870" windowWidth="22875" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -1440,7 +1440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D120"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
       <selection activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>
@@ -2482,8 +2482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A083F05-0FAA-4E78-9E79-0348AF6ADFB8}">
   <dimension ref="A1:D120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added "continue" and "new game" button to reflect progress saving.
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0151F04C-C9C9-497E-A3F0-5FEA3E70A6BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C63D45C-5546-4048-83DD-CDCE2852BDBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5460" yWindow="3870" windowWidth="22875" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="363">
   <si>
     <t>Key</t>
   </si>
@@ -1092,6 +1092,24 @@
   </si>
   <si>
     <t>DISCURSO</t>
+  </si>
+  <si>
+    <t>newGame</t>
+  </si>
+  <si>
+    <t>NEW GAME</t>
+  </si>
+  <si>
+    <t>continue</t>
+  </si>
+  <si>
+    <t>CONTINUE</t>
+  </si>
+  <si>
+    <t>NUEVO JUEGO</t>
+  </si>
+  <si>
+    <t>CONTINUAR</t>
   </si>
 </sst>
 </file>
@@ -1438,10 +1456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D120"/>
+  <dimension ref="A1:D122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="B120" sqref="B120"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2472,6 +2490,22 @@
         <v>355</v>
       </c>
     </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>357</v>
+      </c>
+      <c r="B121" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>359</v>
+      </c>
+      <c r="B122" t="s">
+        <v>360</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2480,10 +2514,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A083F05-0FAA-4E78-9E79-0348AF6ADFB8}">
-  <dimension ref="A1:D120"/>
+  <dimension ref="A1:D122"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3514,6 +3548,22 @@
         <v>356</v>
       </c>
     </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>357</v>
+      </c>
+      <c r="B121" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>359</v>
+      </c>
+      <c r="B122" t="s">
+        <v>362</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added highlight for placement in act 3, show all hints at once.
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C63D45C-5546-4048-83DD-CDCE2852BDBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC0656DA-D11A-49D0-96F0-46B4FA9420CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5460" yWindow="3870" windowWidth="22875" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -719,9 +719,6 @@
     <t>With your knowledge of Newton's law of motion, I am confident that you can accomplish the task!</t>
   </si>
   <si>
-    <t>Press this button to show hints. You can press it again later to show more.</t>
-  </si>
-  <si>
     <t>This block has no wheels. The force of friction will allow the block to resist a certain amount of push or pull from the sides.</t>
   </si>
   <si>
@@ -1073,9 +1070,6 @@
     <t>FINALIZAR</t>
   </si>
   <si>
-    <t>Pulsa este botón para mostrar sugerencias. Puedes volver a presionarlo más tarde para mostrar más.</t>
-  </si>
-  <si>
     <t>Arrastre el control deslizante para observar el movimiento de la rueda a lo largo del tiempo.</t>
   </si>
   <si>
@@ -1110,6 +1104,12 @@
   </si>
   <si>
     <t>CONTINUAR</t>
+  </si>
+  <si>
+    <t>Press this button to show hints.</t>
+  </si>
+  <si>
+    <t>Pulsa este botón para mostrar sugerencias.</t>
   </si>
 </sst>
 </file>
@@ -1458,7 +1458,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
       <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
@@ -1895,7 +1895,7 @@
         <v>213</v>
       </c>
       <c r="B49" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -1991,7 +1991,7 @@
         <v>206</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -2015,7 +2015,7 @@
         <v>211</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -2023,7 +2023,7 @@
         <v>212</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -2047,7 +2047,7 @@
         <v>59</v>
       </c>
       <c r="B68" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -2344,7 +2344,7 @@
         <v>140</v>
       </c>
       <c r="B104" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -2455,7 +2455,7 @@
         <v>209</v>
       </c>
       <c r="B116" t="s">
-        <v>232</v>
+        <v>361</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -2484,26 +2484,26 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B120" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B121" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B122" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -2516,8 +2516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A083F05-0FAA-4E78-9E79-0348AF6ADFB8}">
   <dimension ref="A1:D122"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B122" sqref="B122"/>
+    <sheetView topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2547,7 +2547,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C2">
         <v>1.5</v>
@@ -2561,7 +2561,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2569,7 +2569,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2577,7 +2577,7 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2585,7 +2585,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2593,7 +2593,7 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2601,7 +2601,7 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2609,7 +2609,7 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2617,7 +2617,7 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2633,7 +2633,7 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -2644,7 +2644,7 @@
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -2655,7 +2655,7 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2663,7 +2663,7 @@
         <v>161</v>
       </c>
       <c r="B15" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2671,7 +2671,7 @@
         <v>163</v>
       </c>
       <c r="B16" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2679,7 +2679,7 @@
         <v>159</v>
       </c>
       <c r="B17" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2687,7 +2687,7 @@
         <v>156</v>
       </c>
       <c r="B18" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2695,7 +2695,7 @@
         <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C19">
         <v>1.25</v>
@@ -2706,7 +2706,7 @@
         <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2714,7 +2714,7 @@
         <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2722,7 +2722,7 @@
         <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C22">
         <v>3</v>
@@ -2733,7 +2733,7 @@
         <v>150</v>
       </c>
       <c r="B23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C23">
         <v>1.5</v>
@@ -2744,7 +2744,7 @@
         <v>152</v>
       </c>
       <c r="B24" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C24">
         <v>1.5</v>
@@ -2755,7 +2755,7 @@
         <v>154</v>
       </c>
       <c r="B25" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C25">
         <v>1.5</v>
@@ -2766,7 +2766,7 @@
         <v>31</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -2777,7 +2777,7 @@
         <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -2785,7 +2785,7 @@
         <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2793,7 +2793,7 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -2801,7 +2801,7 @@
         <v>47</v>
       </c>
       <c r="B30" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2809,7 +2809,7 @@
         <v>49</v>
       </c>
       <c r="B31" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2817,7 +2817,7 @@
         <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -2825,7 +2825,7 @@
         <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2833,7 +2833,7 @@
         <v>52</v>
       </c>
       <c r="B34" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2841,7 +2841,7 @@
         <v>54</v>
       </c>
       <c r="B35" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -2849,7 +2849,7 @@
         <v>51</v>
       </c>
       <c r="B36" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2857,7 +2857,7 @@
         <v>79</v>
       </c>
       <c r="B37" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -2865,7 +2865,7 @@
         <v>78</v>
       </c>
       <c r="B38" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -2873,7 +2873,7 @@
         <v>82</v>
       </c>
       <c r="B39" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -2881,7 +2881,7 @@
         <v>185</v>
       </c>
       <c r="B40" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -2889,7 +2889,7 @@
         <v>60</v>
       </c>
       <c r="B41" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -2897,7 +2897,7 @@
         <v>66</v>
       </c>
       <c r="B42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2905,7 +2905,7 @@
         <v>67</v>
       </c>
       <c r="B43" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -2913,7 +2913,7 @@
         <v>68</v>
       </c>
       <c r="B44" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -2921,7 +2921,7 @@
         <v>73</v>
       </c>
       <c r="B45" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -2929,7 +2929,7 @@
         <v>216</v>
       </c>
       <c r="B46" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -2937,7 +2937,7 @@
         <v>72</v>
       </c>
       <c r="B47" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -2945,7 +2945,7 @@
         <v>64</v>
       </c>
       <c r="B48" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -2953,7 +2953,7 @@
         <v>213</v>
       </c>
       <c r="B49" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2961,7 +2961,7 @@
         <v>214</v>
       </c>
       <c r="B50" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2969,7 +2969,7 @@
         <v>37</v>
       </c>
       <c r="B51" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2977,7 +2977,7 @@
         <v>188</v>
       </c>
       <c r="B52" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -2985,7 +2985,7 @@
         <v>189</v>
       </c>
       <c r="B53" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -2993,7 +2993,7 @@
         <v>192</v>
       </c>
       <c r="B54" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -3001,7 +3001,7 @@
         <v>195</v>
       </c>
       <c r="B55" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -3009,7 +3009,7 @@
         <v>196</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -3017,7 +3017,7 @@
         <v>198</v>
       </c>
       <c r="B57" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -3025,7 +3025,7 @@
         <v>200</v>
       </c>
       <c r="B58" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -3033,7 +3033,7 @@
         <v>202</v>
       </c>
       <c r="B59" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -3041,7 +3041,7 @@
         <v>204</v>
       </c>
       <c r="B60" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -3049,7 +3049,7 @@
         <v>206</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -3057,7 +3057,7 @@
         <v>207</v>
       </c>
       <c r="B62" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -3065,7 +3065,7 @@
         <v>56</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -3073,7 +3073,7 @@
         <v>211</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -3081,7 +3081,7 @@
         <v>212</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -3089,7 +3089,7 @@
         <v>57</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -3097,7 +3097,7 @@
         <v>58</v>
       </c>
       <c r="B67" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -3105,7 +3105,7 @@
         <v>59</v>
       </c>
       <c r="B68" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -3113,7 +3113,7 @@
         <v>62</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C69">
         <v>4</v>
@@ -3124,7 +3124,7 @@
         <v>178</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -3132,7 +3132,7 @@
         <v>84</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -3140,7 +3140,7 @@
         <v>86</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -3148,7 +3148,7 @@
         <v>88</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -3156,7 +3156,7 @@
         <v>75</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C74">
         <v>2</v>
@@ -3167,7 +3167,7 @@
         <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -3175,7 +3175,7 @@
         <v>89</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -3183,7 +3183,7 @@
         <v>90</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -3191,7 +3191,7 @@
         <v>120</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -3199,7 +3199,7 @@
         <v>94</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -3207,7 +3207,7 @@
         <v>96</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -3215,7 +3215,7 @@
         <v>100</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -3231,7 +3231,7 @@
         <v>102</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -3239,7 +3239,7 @@
         <v>104</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -3247,7 +3247,7 @@
         <v>115</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -3255,7 +3255,7 @@
         <v>106</v>
       </c>
       <c r="B86" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -3263,7 +3263,7 @@
         <v>108</v>
       </c>
       <c r="B87" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -3271,7 +3271,7 @@
         <v>109</v>
       </c>
       <c r="B88" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -3279,7 +3279,7 @@
         <v>117</v>
       </c>
       <c r="B89" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -3287,7 +3287,7 @@
         <v>110</v>
       </c>
       <c r="B90" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -3295,7 +3295,7 @@
         <v>111</v>
       </c>
       <c r="B91" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -3303,7 +3303,7 @@
         <v>112</v>
       </c>
       <c r="B92" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -3311,7 +3311,7 @@
         <v>113</v>
       </c>
       <c r="B93" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -3319,7 +3319,7 @@
         <v>123</v>
       </c>
       <c r="B94" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -3327,7 +3327,7 @@
         <v>125</v>
       </c>
       <c r="B95" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -3335,7 +3335,7 @@
         <v>126</v>
       </c>
       <c r="B96" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -3343,7 +3343,7 @@
         <v>114</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -3351,7 +3351,7 @@
         <v>129</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -3359,7 +3359,7 @@
         <v>130</v>
       </c>
       <c r="B99" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C99">
         <v>3</v>
@@ -3370,7 +3370,7 @@
         <v>134</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -3378,7 +3378,7 @@
         <v>136</v>
       </c>
       <c r="B101" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -3386,7 +3386,7 @@
         <v>137</v>
       </c>
       <c r="B102" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -3394,7 +3394,7 @@
         <v>138</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -3402,7 +3402,7 @@
         <v>140</v>
       </c>
       <c r="B104" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -3410,7 +3410,7 @@
         <v>141</v>
       </c>
       <c r="B105" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -3418,7 +3418,7 @@
         <v>142</v>
       </c>
       <c r="B106" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C106">
         <v>3</v>
@@ -3429,7 +3429,7 @@
         <v>145</v>
       </c>
       <c r="B107" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C107">
         <v>3</v>
@@ -3440,7 +3440,7 @@
         <v>147</v>
       </c>
       <c r="B108" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -3448,7 +3448,7 @@
         <v>165</v>
       </c>
       <c r="B109" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C109">
         <v>2</v>
@@ -3459,7 +3459,7 @@
         <v>168</v>
       </c>
       <c r="B110" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -3467,7 +3467,7 @@
         <v>170</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -3475,7 +3475,7 @@
         <v>230</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -3483,7 +3483,7 @@
         <v>171</v>
       </c>
       <c r="B113" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C113">
         <v>2</v>
@@ -3494,7 +3494,7 @@
         <v>172</v>
       </c>
       <c r="B114" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C114">
         <v>3</v>
@@ -3505,7 +3505,7 @@
         <v>174</v>
       </c>
       <c r="B115" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -3513,7 +3513,7 @@
         <v>209</v>
       </c>
       <c r="B116" t="s">
-        <v>350</v>
+        <v>362</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -3521,7 +3521,7 @@
         <v>218</v>
       </c>
       <c r="B117" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -3529,7 +3529,7 @@
         <v>224</v>
       </c>
       <c r="B118" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -3537,31 +3537,31 @@
         <v>227</v>
       </c>
       <c r="B119" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
+        <v>352</v>
+      </c>
+      <c r="B120" t="s">
         <v>354</v>
-      </c>
-      <c r="B120" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B121" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B122" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added some simple intro to act 3-1
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC0656DA-D11A-49D0-96F0-46B4FA9420CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E345CE-87C2-4D86-8683-F9899BB27142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5460" yWindow="3870" windowWidth="22875" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="371">
   <si>
     <t>Key</t>
   </si>
@@ -1110,6 +1110,30 @@
   </si>
   <si>
     <t>Pulsa este botón para mostrar sugerencias.</t>
+  </si>
+  <si>
+    <t>act_3_intro_1</t>
+  </si>
+  <si>
+    <t>act_3_intro_2</t>
+  </si>
+  <si>
+    <t>act_3_intro_3</t>
+  </si>
+  <si>
+    <t>act_3_intro_4</t>
+  </si>
+  <si>
+    <t>In this act, we will be guiding the golden ball to its holy source.</t>
+  </si>
+  <si>
+    <t>To do that, you must place force fields to influence the golden ball’s movement.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remember that so long as any forces are acting on an object, its acceleration will change. Thus, causing the object’s speed to change over time. </t>
+  </si>
+  <si>
+    <t>Now go forth, and attach a force field on the wall to get the ball rolling!</t>
   </si>
 </sst>
 </file>
@@ -1456,10 +1480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D122"/>
+  <dimension ref="A1:D126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B116" sqref="B116"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2506,18 +2530,50 @@
         <v>358</v>
       </c>
     </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>363</v>
+      </c>
+      <c r="B123" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>364</v>
+      </c>
+      <c r="B124" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>365</v>
+      </c>
+      <c r="B125" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>366</v>
+      </c>
+      <c r="B126" t="s">
+        <v>370</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A083F05-0FAA-4E78-9E79-0348AF6ADFB8}">
-  <dimension ref="A1:D122"/>
+  <dimension ref="A1:D126"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B116" sqref="B116"/>
+    <sheetView topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="B123" sqref="B123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3564,6 +3620,26 @@
         <v>360</v>
       </c>
     </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>366</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
more dialogs: act 3-2, 3-3
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E345CE-87C2-4D86-8683-F9899BB27142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17384EB6-8F60-4346-99DB-04BDEB40BE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5460" yWindow="3870" windowWidth="22875" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="385">
   <si>
     <t>Key</t>
   </si>
@@ -1134,6 +1134,48 @@
   </si>
   <si>
     <t>Now go forth, and attach a force field on the wall to get the ball rolling!</t>
+  </si>
+  <si>
+    <t>act_3_2_intro_1</t>
+  </si>
+  <si>
+    <t>act_3_2_intro_2</t>
+  </si>
+  <si>
+    <t>act_3_2_intro_3</t>
+  </si>
+  <si>
+    <t>This time around, we will be placing two force fields.</t>
+  </si>
+  <si>
+    <t>In order to allow the golden ball to take flight, one must counteract the gravitational force with a much greater force.</t>
+  </si>
+  <si>
+    <t>Please take note of the force field’s direction when placing them on the wall. Good luck!</t>
+  </si>
+  <si>
+    <t>act_3_3_intro_1</t>
+  </si>
+  <si>
+    <t>act_3_3_intro_2</t>
+  </si>
+  <si>
+    <t>act_3_3_intro_3</t>
+  </si>
+  <si>
+    <t>act_3_3_intro_4</t>
+  </si>
+  <si>
+    <t>First: An object at rest will remain at rest, and an object in motion will maintain a constant velocity unless acted upon by a net external force.</t>
+  </si>
+  <si>
+    <t>Second: The acceleration of an object is proportional to the net force acting on it, and inversely proportional to its mass.</t>
+  </si>
+  <si>
+    <t>Keep these in mind, and you will surely be a force to be reckoned with!</t>
+  </si>
+  <si>
+    <t>Now that you’ve come this far, it’s all up to you! Remember all that you’ve learned about Newton’s first two laws.</t>
   </si>
 </sst>
 </file>
@@ -1480,10 +1522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D126"/>
+  <dimension ref="A1:D133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="B122" sqref="B122"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="B130" sqref="B130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2562,6 +2604,62 @@
         <v>370</v>
       </c>
     </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>371</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>372</v>
+      </c>
+      <c r="B128" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>373</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>377</v>
+      </c>
+      <c r="B130" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>378</v>
+      </c>
+      <c r="B131" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>379</v>
+      </c>
+      <c r="B132" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>380</v>
+      </c>
+      <c r="B133" t="s">
+        <v>383</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -2570,7 +2668,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A083F05-0FAA-4E78-9E79-0348AF6ADFB8}">
-  <dimension ref="A1:D126"/>
+  <dimension ref="A1:D129"/>
   <sheetViews>
     <sheetView topLeftCell="A100" workbookViewId="0">
       <selection activeCell="B123" sqref="B123"/>
@@ -3640,6 +3738,21 @@
         <v>366</v>
       </c>
     </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>373</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update graph explanation text, make act 2-1 a little more interesting
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17384EB6-8F60-4346-99DB-04BDEB40BE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E2A40B-2499-46B5-87EC-CDF12C7BF2C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5460" yWindow="3870" windowWidth="22875" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5700" yWindow="3795" windowWidth="22875" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="384">
   <si>
     <t>Key</t>
   </si>
@@ -395,9 +395,6 @@
     <t>newton_second_law_graph_1</t>
   </si>
   <si>
-    <t>The graph maps out the trails across time along the x and y axis. Be sure to check the velocity and acceleration by scrolling down.</t>
-  </si>
-  <si>
     <t>newton_second_law_graph_2</t>
   </si>
   <si>
@@ -1004,9 +1001,6 @@
     <t>A medida que cae la rueda, la velocidad en el eje Y comienza a disminuir.</t>
   </si>
   <si>
-    <t>El gráfico asigna los senderos a lo largo del tiempo a lo largo de los ejes x e y. Asegúrese de comprobar la velocidad y la aceleración desplazándose hacia abajo.</t>
-  </si>
-  <si>
     <t>Observe cómo se curva la línea de posición a medida que aumenta la velocidad, lo que indica que hay aceleración.</t>
   </si>
   <si>
@@ -1176,6 +1170,9 @@
   </si>
   <si>
     <t>Now that you’ve come this far, it’s all up to you! Remember all that you’ve learned about Newton’s first two laws.</t>
+  </si>
+  <si>
+    <t>The graph maps out the trails across time along the x and y axis. Check out the velocity and acceleration by pressing the tabs above the graph.</t>
   </si>
 </sst>
 </file>
@@ -1524,8 +1521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="B130" sqref="B130"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1569,7 +1566,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1668,34 +1665,34 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>160</v>
+      </c>
+      <c r="B15" t="s">
         <v>161</v>
-      </c>
-      <c r="B15" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>162</v>
+      </c>
+      <c r="B16" t="s">
         <v>163</v>
-      </c>
-      <c r="B16" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>158</v>
+      </c>
+      <c r="B17" t="s">
         <v>159</v>
-      </c>
-      <c r="B17" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>155</v>
+      </c>
+      <c r="B18" t="s">
         <v>156</v>
-      </c>
-      <c r="B18" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1730,7 +1727,7 @@
         <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C22">
         <v>3</v>
@@ -1738,10 +1735,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>149</v>
+      </c>
+      <c r="B23" t="s">
         <v>150</v>
-      </c>
-      <c r="B23" t="s">
-        <v>151</v>
       </c>
       <c r="C23">
         <v>1.5</v>
@@ -1749,10 +1746,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>151</v>
+      </c>
+      <c r="B24" t="s">
         <v>152</v>
-      </c>
-      <c r="B24" t="s">
-        <v>153</v>
       </c>
       <c r="C24">
         <v>1.5</v>
@@ -1760,10 +1757,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>153</v>
+      </c>
+      <c r="B25" t="s">
         <v>154</v>
-      </c>
-      <c r="B25" t="s">
-        <v>155</v>
       </c>
       <c r="C25">
         <v>1.5</v>
@@ -1833,7 +1830,7 @@
         <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1857,7 +1854,7 @@
         <v>51</v>
       </c>
       <c r="B36" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1886,10 +1883,10 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>184</v>
+      </c>
+      <c r="B40" t="s">
         <v>185</v>
-      </c>
-      <c r="B40" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1934,10 +1931,10 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B46" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1958,18 +1955,18 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B49" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>213</v>
+      </c>
+      <c r="B50" t="s">
         <v>214</v>
-      </c>
-      <c r="B50" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1977,95 +1974,95 @@
         <v>37</v>
       </c>
       <c r="B51" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B52" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B53" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>191</v>
+      </c>
+      <c r="B54" t="s">
         <v>192</v>
-      </c>
-      <c r="B54" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B55" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>195</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B57" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>199</v>
+      </c>
+      <c r="B58" t="s">
         <v>200</v>
-      </c>
-      <c r="B58" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>201</v>
+      </c>
+      <c r="B59" t="s">
         <v>202</v>
-      </c>
-      <c r="B59" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>203</v>
+      </c>
+      <c r="B60" t="s">
         <v>204</v>
-      </c>
-      <c r="B60" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>206</v>
+      </c>
+      <c r="B62" t="s">
         <v>207</v>
-      </c>
-      <c r="B62" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -2073,23 +2070,23 @@
         <v>56</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -2097,7 +2094,7 @@
         <v>57</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -2105,7 +2102,7 @@
         <v>58</v>
       </c>
       <c r="B67" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -2113,7 +2110,7 @@
         <v>59</v>
       </c>
       <c r="B68" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -2129,10 +2126,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>177</v>
+      </c>
+      <c r="B70" s="4" t="s">
         <v>178</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -2175,7 +2172,7 @@
         <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -2287,7 +2284,7 @@
         <v>117</v>
       </c>
       <c r="B89" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -2295,7 +2292,7 @@
         <v>110</v>
       </c>
       <c r="B90" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -2303,7 +2300,7 @@
         <v>111</v>
       </c>
       <c r="B91" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -2311,7 +2308,7 @@
         <v>112</v>
       </c>
       <c r="B92" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -2319,7 +2316,7 @@
         <v>113</v>
       </c>
       <c r="B93" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -2327,23 +2324,23 @@
         <v>123</v>
       </c>
       <c r="B94" t="s">
-        <v>124</v>
+        <v>383</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B95" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B96" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -2351,23 +2348,23 @@
         <v>114</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>129</v>
+      </c>
+      <c r="B99" t="s">
         <v>130</v>
-      </c>
-      <c r="B99" t="s">
-        <v>131</v>
       </c>
       <c r="C99">
         <v>3</v>
@@ -2375,58 +2372,58 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B101" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B102" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
+        <v>137</v>
+      </c>
+      <c r="B103" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B104" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B105" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
+        <v>141</v>
+      </c>
+      <c r="B106" t="s">
         <v>142</v>
-      </c>
-      <c r="B106" t="s">
-        <v>143</v>
       </c>
       <c r="C106">
         <v>3</v>
@@ -2434,10 +2431,10 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
+        <v>144</v>
+      </c>
+      <c r="B107" t="s">
         <v>145</v>
-      </c>
-      <c r="B107" t="s">
-        <v>146</v>
       </c>
       <c r="C107">
         <v>3</v>
@@ -2445,18 +2442,18 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
+        <v>146</v>
+      </c>
+      <c r="B108" t="s">
         <v>147</v>
-      </c>
-      <c r="B108" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
+        <v>164</v>
+      </c>
+      <c r="B109" t="s">
         <v>165</v>
-      </c>
-      <c r="B109" t="s">
-        <v>166</v>
       </c>
       <c r="C109">
         <v>2</v>
@@ -2464,34 +2461,34 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B110" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
+        <v>229</v>
+      </c>
+      <c r="B112" s="2" t="s">
         <v>230</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B113" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C113">
         <v>2</v>
@@ -2499,10 +2496,10 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
+        <v>171</v>
+      </c>
+      <c r="B114" t="s">
         <v>172</v>
-      </c>
-      <c r="B114" t="s">
-        <v>173</v>
       </c>
       <c r="C114">
         <v>3</v>
@@ -2510,154 +2507,154 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
+        <v>173</v>
+      </c>
+      <c r="B115" t="s">
         <v>174</v>
-      </c>
-      <c r="B115" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B116" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B117" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
+        <v>223</v>
+      </c>
+      <c r="B118" t="s">
         <v>224</v>
-      </c>
-      <c r="B118" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
+        <v>226</v>
+      </c>
+      <c r="B119" t="s">
         <v>227</v>
-      </c>
-      <c r="B119" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B120" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B121" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B122" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B123" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B124" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B125" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B126" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B128" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B130" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B131" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B132" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B133" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>
@@ -2670,8 +2667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A083F05-0FAA-4E78-9E79-0348AF6ADFB8}">
   <dimension ref="A1:D129"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="B123" sqref="B123"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2701,7 +2698,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C2">
         <v>1.5</v>
@@ -2715,7 +2712,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2723,7 +2720,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2731,7 +2728,7 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2739,7 +2736,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2747,7 +2744,7 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2755,7 +2752,7 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2763,7 +2760,7 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2771,7 +2768,7 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2787,7 +2784,7 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -2798,7 +2795,7 @@
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -2809,39 +2806,39 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B15" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B16" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B17" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2849,7 +2846,7 @@
         <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C19">
         <v>1.25</v>
@@ -2860,7 +2857,7 @@
         <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2868,7 +2865,7 @@
         <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2876,7 +2873,7 @@
         <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C22">
         <v>3</v>
@@ -2884,10 +2881,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C23">
         <v>1.5</v>
@@ -2895,10 +2892,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C24">
         <v>1.5</v>
@@ -2906,10 +2903,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B25" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C25">
         <v>1.5</v>
@@ -2920,7 +2917,7 @@
         <v>31</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -2931,7 +2928,7 @@
         <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -2939,7 +2936,7 @@
         <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2947,7 +2944,7 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -2955,7 +2952,7 @@
         <v>47</v>
       </c>
       <c r="B30" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2963,7 +2960,7 @@
         <v>49</v>
       </c>
       <c r="B31" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2971,7 +2968,7 @@
         <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -2979,7 +2976,7 @@
         <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2987,7 +2984,7 @@
         <v>52</v>
       </c>
       <c r="B34" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2995,7 +2992,7 @@
         <v>54</v>
       </c>
       <c r="B35" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -3003,7 +3000,7 @@
         <v>51</v>
       </c>
       <c r="B36" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -3011,7 +3008,7 @@
         <v>79</v>
       </c>
       <c r="B37" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -3019,7 +3016,7 @@
         <v>78</v>
       </c>
       <c r="B38" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -3027,15 +3024,15 @@
         <v>82</v>
       </c>
       <c r="B39" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B40" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -3043,7 +3040,7 @@
         <v>60</v>
       </c>
       <c r="B41" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -3051,7 +3048,7 @@
         <v>66</v>
       </c>
       <c r="B42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -3059,7 +3056,7 @@
         <v>67</v>
       </c>
       <c r="B43" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -3067,7 +3064,7 @@
         <v>68</v>
       </c>
       <c r="B44" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -3075,15 +3072,15 @@
         <v>73</v>
       </c>
       <c r="B45" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B46" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -3091,7 +3088,7 @@
         <v>72</v>
       </c>
       <c r="B47" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -3099,23 +3096,23 @@
         <v>64</v>
       </c>
       <c r="B48" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B49" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B50" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -3123,95 +3120,95 @@
         <v>37</v>
       </c>
       <c r="B51" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B52" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B53" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B54" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B55" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B57" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B58" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B59" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B60" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B62" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -3219,23 +3216,23 @@
         <v>56</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -3243,7 +3240,7 @@
         <v>57</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -3251,7 +3248,7 @@
         <v>58</v>
       </c>
       <c r="B67" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -3259,7 +3256,7 @@
         <v>59</v>
       </c>
       <c r="B68" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -3267,7 +3264,7 @@
         <v>62</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C69">
         <v>4</v>
@@ -3275,10 +3272,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -3286,7 +3283,7 @@
         <v>84</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -3294,7 +3291,7 @@
         <v>86</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -3302,7 +3299,7 @@
         <v>88</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -3310,7 +3307,7 @@
         <v>75</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C74">
         <v>2</v>
@@ -3321,7 +3318,7 @@
         <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -3329,7 +3326,7 @@
         <v>89</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -3337,7 +3334,7 @@
         <v>90</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -3345,7 +3342,7 @@
         <v>120</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -3353,7 +3350,7 @@
         <v>94</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -3361,7 +3358,7 @@
         <v>96</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -3369,7 +3366,7 @@
         <v>100</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -3385,7 +3382,7 @@
         <v>102</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -3393,7 +3390,7 @@
         <v>104</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -3401,7 +3398,7 @@
         <v>115</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -3409,7 +3406,7 @@
         <v>106</v>
       </c>
       <c r="B86" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -3417,7 +3414,7 @@
         <v>108</v>
       </c>
       <c r="B87" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -3425,7 +3422,7 @@
         <v>109</v>
       </c>
       <c r="B88" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -3433,7 +3430,7 @@
         <v>117</v>
       </c>
       <c r="B89" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -3441,7 +3438,7 @@
         <v>110</v>
       </c>
       <c r="B90" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -3449,7 +3446,7 @@
         <v>111</v>
       </c>
       <c r="B91" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -3457,7 +3454,7 @@
         <v>112</v>
       </c>
       <c r="B92" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -3465,31 +3462,28 @@
         <v>113</v>
       </c>
       <c r="B93" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>123</v>
       </c>
-      <c r="B94" t="s">
-        <v>327</v>
-      </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B95" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B96" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -3497,23 +3491,23 @@
         <v>114</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B99" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C99">
         <v>3</v>
@@ -3521,58 +3515,58 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B101" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B102" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B104" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B105" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B106" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C106">
         <v>3</v>
@@ -3580,10 +3574,10 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B107" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C107">
         <v>3</v>
@@ -3591,18 +3585,18 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B108" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B109" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C109">
         <v>2</v>
@@ -3610,34 +3604,34 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B110" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B113" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C113">
         <v>2</v>
@@ -3645,10 +3639,10 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B114" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C114">
         <v>3</v>
@@ -3656,101 +3650,101 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B115" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B116" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B117" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B118" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B119" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
+        <v>350</v>
+      </c>
+      <c r="B120" t="s">
         <v>352</v>
-      </c>
-      <c r="B120" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B121" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B122" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add telemetry hint for first target in act 2-2, some tweaks to intro dialog in act 2-2
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E2A40B-2499-46B5-87EC-CDF12C7BF2C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABBA3CC7-4ECC-4A25-98FD-EE45C51C8509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5700" yWindow="3795" windowWidth="22875" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="387">
   <si>
     <t>Key</t>
   </si>
@@ -527,9 +527,6 @@
     <t>act_2_end_dlg_1</t>
   </si>
   <si>
-    <t>Drag this to adjust the cannon's angle.</t>
-  </si>
-  <si>
     <t>act_2_end_dlg_2</t>
   </si>
   <si>
@@ -722,9 +719,6 @@
     <t>Here's a locked treasure chest as a demonstration. Put the correct amount of weight on the other platform to unlock it!</t>
   </si>
   <si>
-    <t>The cannon can launch projectiles at different directions by adjusting its angle. This will allow us to hit targets at various heights.</t>
-  </si>
-  <si>
     <t>Inertia is proportional to Mass</t>
   </si>
   <si>
@@ -1016,9 +1010,6 @@
     <t>Objetivos eliminados</t>
   </si>
   <si>
-    <t>Arrastra esto para guiar el ángulo del cañón.</t>
-  </si>
-  <si>
     <t>Recuerda revisar el gráfico para analizar la trayectoria de la bala de cañón.</t>
   </si>
   <si>
@@ -1028,9 +1019,6 @@
     <t>¡Vamos a sacar el poderoso cañón para vencer a estas alimañas!</t>
   </si>
   <si>
-    <t>El cañón puede lanzar proyectiles en diferentes direcciones ajustando su ángulo. Esto nos permitirá alcanzar objetivos a distintas alturas.</t>
-  </si>
-  <si>
     <t>Arrastre el campo de fuerza a esta superficie.</t>
   </si>
   <si>
@@ -1173,6 +1161,27 @@
   </si>
   <si>
     <t>The graph maps out the trails across time along the x and y axis. Check out the velocity and acceleration by pressing the tabs above the graph.</t>
+  </si>
+  <si>
+    <t>newton_second_law_2_dlg_4</t>
+  </si>
+  <si>
+    <t>This time around, we will be able to adjust the direction of the force upwards to counteract the gravitational force.</t>
+  </si>
+  <si>
+    <t>Now let's adjust the cannon's angle and blast force to hit the nearest goblin.</t>
+  </si>
+  <si>
+    <t>act_2_2_force_hint</t>
+  </si>
+  <si>
+    <t>Drag this to adjust the cannon's angle to 70°.</t>
+  </si>
+  <si>
+    <t>Set the force value to 310N.</t>
+  </si>
+  <si>
+    <t>Arrastra esto para guiar el ángulo del cañón a 70°.</t>
   </si>
 </sst>
 </file>
@@ -1519,10 +1528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D133"/>
+  <dimension ref="A1:D135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1830,7 +1839,7 @@
         <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1854,7 +1863,7 @@
         <v>51</v>
       </c>
       <c r="B36" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1883,10 +1892,10 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>183</v>
+      </c>
+      <c r="B40" t="s">
         <v>184</v>
-      </c>
-      <c r="B40" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1931,10 +1940,10 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B46" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1955,18 +1964,18 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B49" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>212</v>
+      </c>
+      <c r="B50" t="s">
         <v>213</v>
-      </c>
-      <c r="B50" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1974,95 +1983,95 @@
         <v>37</v>
       </c>
       <c r="B51" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B52" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B53" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>190</v>
+      </c>
+      <c r="B54" t="s">
         <v>191</v>
-      </c>
-      <c r="B54" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B55" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>194</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>195</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B57" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>198</v>
+      </c>
+      <c r="B58" t="s">
         <v>199</v>
-      </c>
-      <c r="B58" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>200</v>
+      </c>
+      <c r="B59" t="s">
         <v>201</v>
-      </c>
-      <c r="B59" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>202</v>
+      </c>
+      <c r="B60" t="s">
         <v>203</v>
-      </c>
-      <c r="B60" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>205</v>
+      </c>
+      <c r="B62" t="s">
         <v>206</v>
-      </c>
-      <c r="B62" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -2070,23 +2079,23 @@
         <v>56</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -2094,7 +2103,7 @@
         <v>57</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -2102,7 +2111,7 @@
         <v>58</v>
       </c>
       <c r="B67" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -2110,7 +2119,7 @@
         <v>59</v>
       </c>
       <c r="B68" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -2126,10 +2135,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>176</v>
+      </c>
+      <c r="B70" s="4" t="s">
         <v>177</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -2182,6 +2191,9 @@
       <c r="B76" s="4" t="s">
         <v>92</v>
       </c>
+      <c r="C76">
+        <v>4</v>
+      </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
@@ -2284,7 +2296,7 @@
         <v>117</v>
       </c>
       <c r="B89" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -2292,7 +2304,7 @@
         <v>110</v>
       </c>
       <c r="B90" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -2300,7 +2312,7 @@
         <v>111</v>
       </c>
       <c r="B91" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -2308,7 +2320,7 @@
         <v>112</v>
       </c>
       <c r="B92" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -2316,7 +2328,7 @@
         <v>113</v>
       </c>
       <c r="B93" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -2324,7 +2336,7 @@
         <v>123</v>
       </c>
       <c r="B94" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -2348,7 +2360,7 @@
         <v>114</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -2375,286 +2387,308 @@
         <v>133</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>168</v>
+        <v>384</v>
+      </c>
+      <c r="C100">
+        <v>4</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>135</v>
-      </c>
-      <c r="B101" t="s">
-        <v>134</v>
+        <v>383</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="C101">
+        <v>4</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B102" t="s">
-        <v>157</v>
+        <v>134</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>137</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
+      </c>
+      <c r="B103" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>139</v>
-      </c>
-      <c r="B104" t="s">
-        <v>233</v>
+        <v>137</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>140</v>
-      </c>
-      <c r="B105" t="s">
-        <v>143</v>
+        <v>380</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B106" t="s">
-        <v>142</v>
-      </c>
-      <c r="C106">
-        <v>3</v>
+        <v>382</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B107" t="s">
-        <v>145</v>
-      </c>
-      <c r="C107">
-        <v>3</v>
+        <v>143</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B108" t="s">
-        <v>147</v>
+        <v>142</v>
+      </c>
+      <c r="C108">
+        <v>3</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="B109" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="C109">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="B110" t="s">
-        <v>228</v>
+        <v>147</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>169</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>181</v>
+        <v>164</v>
+      </c>
+      <c r="B111" t="s">
+        <v>165</v>
+      </c>
+      <c r="C111">
+        <v>2</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>229</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>230</v>
+        <v>167</v>
+      </c>
+      <c r="B112" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>170</v>
-      </c>
-      <c r="B113" t="s">
-        <v>183</v>
-      </c>
-      <c r="C113">
-        <v>2</v>
+        <v>168</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>171</v>
-      </c>
-      <c r="B114" t="s">
-        <v>172</v>
-      </c>
-      <c r="C114">
-        <v>3</v>
+        <v>228</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B115" t="s">
-        <v>174</v>
+        <v>182</v>
+      </c>
+      <c r="C115">
+        <v>2</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>208</v>
+        <v>170</v>
       </c>
       <c r="B116" t="s">
-        <v>359</v>
+        <v>171</v>
+      </c>
+      <c r="C116">
+        <v>3</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>217</v>
+        <v>172</v>
       </c>
       <c r="B117" t="s">
-        <v>216</v>
+        <v>173</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="B118" t="s">
-        <v>224</v>
+        <v>355</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="B119" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>350</v>
+        <v>222</v>
       </c>
       <c r="B120" t="s">
-        <v>351</v>
+        <v>223</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>353</v>
+        <v>225</v>
       </c>
       <c r="B121" t="s">
-        <v>354</v>
+        <v>226</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="B122" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
       <c r="B123" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
       <c r="B124" t="s">
-        <v>366</v>
+        <v>352</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="B125" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="B126" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>369</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>372</v>
+        <v>359</v>
+      </c>
+      <c r="B127" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="B128" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="B130" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>376</v>
-      </c>
-      <c r="B131" t="s">
-        <v>379</v>
+        <v>367</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="B132" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="B133" t="s">
-        <v>381</v>
+        <v>375</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>373</v>
+      </c>
+      <c r="B134" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>374</v>
+      </c>
+      <c r="B135" t="s">
+        <v>377</v>
       </c>
     </row>
   </sheetData>
@@ -2665,10 +2699,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A083F05-0FAA-4E78-9E79-0348AF6ADFB8}">
-  <dimension ref="A1:D129"/>
+  <dimension ref="A1:D131"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2698,7 +2732,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C2">
         <v>1.5</v>
@@ -2712,7 +2746,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2720,7 +2754,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2728,7 +2762,7 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2736,7 +2770,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2744,7 +2778,7 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2752,7 +2786,7 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2760,7 +2794,7 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2768,7 +2802,7 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2784,7 +2818,7 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -2795,7 +2829,7 @@
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -2806,7 +2840,7 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2814,7 +2848,7 @@
         <v>160</v>
       </c>
       <c r="B15" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2822,7 +2856,7 @@
         <v>162</v>
       </c>
       <c r="B16" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2830,7 +2864,7 @@
         <v>158</v>
       </c>
       <c r="B17" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2838,7 +2872,7 @@
         <v>155</v>
       </c>
       <c r="B18" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2846,7 +2880,7 @@
         <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C19">
         <v>1.25</v>
@@ -2857,7 +2891,7 @@
         <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2865,7 +2899,7 @@
         <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2873,7 +2907,7 @@
         <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C22">
         <v>3</v>
@@ -2884,7 +2918,7 @@
         <v>149</v>
       </c>
       <c r="B23" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C23">
         <v>1.5</v>
@@ -2895,7 +2929,7 @@
         <v>151</v>
       </c>
       <c r="B24" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C24">
         <v>1.5</v>
@@ -2906,7 +2940,7 @@
         <v>153</v>
       </c>
       <c r="B25" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C25">
         <v>1.5</v>
@@ -2917,7 +2951,7 @@
         <v>31</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -2928,7 +2962,7 @@
         <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -2936,7 +2970,7 @@
         <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2944,7 +2978,7 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -2952,7 +2986,7 @@
         <v>47</v>
       </c>
       <c r="B30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2960,7 +2994,7 @@
         <v>49</v>
       </c>
       <c r="B31" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2968,7 +3002,7 @@
         <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -2976,7 +3010,7 @@
         <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2984,7 +3018,7 @@
         <v>52</v>
       </c>
       <c r="B34" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2992,7 +3026,7 @@
         <v>54</v>
       </c>
       <c r="B35" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -3000,7 +3034,7 @@
         <v>51</v>
       </c>
       <c r="B36" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -3008,7 +3042,7 @@
         <v>79</v>
       </c>
       <c r="B37" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -3016,7 +3050,7 @@
         <v>78</v>
       </c>
       <c r="B38" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -3024,15 +3058,15 @@
         <v>82</v>
       </c>
       <c r="B39" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B40" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -3040,7 +3074,7 @@
         <v>60</v>
       </c>
       <c r="B41" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -3048,7 +3082,7 @@
         <v>66</v>
       </c>
       <c r="B42" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -3056,7 +3090,7 @@
         <v>67</v>
       </c>
       <c r="B43" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -3064,7 +3098,7 @@
         <v>68</v>
       </c>
       <c r="B44" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -3072,15 +3106,15 @@
         <v>73</v>
       </c>
       <c r="B45" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B46" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -3088,7 +3122,7 @@
         <v>72</v>
       </c>
       <c r="B47" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -3096,23 +3130,23 @@
         <v>64</v>
       </c>
       <c r="B48" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B49" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B50" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -3120,95 +3154,95 @@
         <v>37</v>
       </c>
       <c r="B51" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B52" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B53" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B54" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B55" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B57" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B58" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B59" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B60" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B62" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -3216,23 +3250,23 @@
         <v>56</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -3240,7 +3274,7 @@
         <v>57</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -3248,7 +3282,7 @@
         <v>58</v>
       </c>
       <c r="B67" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -3256,7 +3290,7 @@
         <v>59</v>
       </c>
       <c r="B68" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -3264,7 +3298,7 @@
         <v>62</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C69">
         <v>4</v>
@@ -3272,10 +3306,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -3283,7 +3317,7 @@
         <v>84</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -3291,7 +3325,7 @@
         <v>86</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -3299,7 +3333,7 @@
         <v>88</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -3307,7 +3341,7 @@
         <v>75</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C74">
         <v>2</v>
@@ -3318,7 +3352,7 @@
         <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -3326,7 +3360,10 @@
         <v>89</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>309</v>
+        <v>307</v>
+      </c>
+      <c r="C76">
+        <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -3334,7 +3371,7 @@
         <v>90</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -3342,7 +3379,7 @@
         <v>120</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -3350,7 +3387,7 @@
         <v>94</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -3358,7 +3395,7 @@
         <v>96</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -3366,7 +3403,7 @@
         <v>100</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -3382,7 +3419,7 @@
         <v>102</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -3390,7 +3427,7 @@
         <v>104</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -3398,7 +3435,7 @@
         <v>115</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -3406,7 +3443,7 @@
         <v>106</v>
       </c>
       <c r="B86" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -3414,7 +3451,7 @@
         <v>108</v>
       </c>
       <c r="B87" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -3422,7 +3459,7 @@
         <v>109</v>
       </c>
       <c r="B88" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -3430,7 +3467,7 @@
         <v>117</v>
       </c>
       <c r="B89" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -3438,7 +3475,7 @@
         <v>110</v>
       </c>
       <c r="B90" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -3446,7 +3483,7 @@
         <v>111</v>
       </c>
       <c r="B91" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -3454,7 +3491,7 @@
         <v>112</v>
       </c>
       <c r="B92" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -3462,7 +3499,7 @@
         <v>113</v>
       </c>
       <c r="B93" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -3475,7 +3512,7 @@
         <v>124</v>
       </c>
       <c r="B95" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -3483,7 +3520,7 @@
         <v>125</v>
       </c>
       <c r="B96" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -3491,7 +3528,7 @@
         <v>114</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -3499,7 +3536,7 @@
         <v>128</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -3507,7 +3544,7 @@
         <v>129</v>
       </c>
       <c r="B99" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C99">
         <v>3</v>
@@ -3518,233 +3555,248 @@
         <v>133</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>331</v>
+        <v>386</v>
+      </c>
+      <c r="C100">
+        <v>4</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>135</v>
-      </c>
-      <c r="B101" t="s">
-        <v>332</v>
+        <v>383</v>
+      </c>
+      <c r="B101" s="2"/>
+      <c r="C101">
+        <v>4</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B102" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>137</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>334</v>
+        <v>136</v>
+      </c>
+      <c r="B103" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>139</v>
-      </c>
-      <c r="B104" t="s">
-        <v>335</v>
+        <v>137</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>140</v>
-      </c>
-      <c r="B105" t="s">
-        <v>336</v>
-      </c>
+        <v>380</v>
+      </c>
+      <c r="B105" s="2"/>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>141</v>
-      </c>
-      <c r="B106" t="s">
-        <v>337</v>
-      </c>
-      <c r="C106">
-        <v>3</v>
+        <v>139</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B107" t="s">
-        <v>338</v>
-      </c>
-      <c r="C107">
-        <v>3</v>
+        <v>332</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B108" t="s">
-        <v>339</v>
+        <v>333</v>
+      </c>
+      <c r="C108">
+        <v>3</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="B109" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="C109">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="B110" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>169</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>342</v>
+        <v>164</v>
+      </c>
+      <c r="B111" t="s">
+        <v>336</v>
+      </c>
+      <c r="C111">
+        <v>2</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>229</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>343</v>
+        <v>167</v>
+      </c>
+      <c r="B112" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>170</v>
-      </c>
-      <c r="B113" t="s">
-        <v>344</v>
-      </c>
-      <c r="C113">
-        <v>2</v>
+        <v>168</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>171</v>
-      </c>
-      <c r="B114" t="s">
-        <v>345</v>
-      </c>
-      <c r="C114">
-        <v>3</v>
+        <v>228</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B115" t="s">
-        <v>346</v>
+        <v>340</v>
+      </c>
+      <c r="C115">
+        <v>2</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>208</v>
+        <v>170</v>
       </c>
       <c r="B116" t="s">
-        <v>360</v>
+        <v>341</v>
+      </c>
+      <c r="C116">
+        <v>3</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>217</v>
+        <v>172</v>
       </c>
       <c r="B117" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="B118" t="s">
-        <v>348</v>
+        <v>356</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="B119" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>350</v>
+        <v>222</v>
       </c>
       <c r="B120" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>353</v>
+        <v>225</v>
       </c>
       <c r="B121" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="B122" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>361</v>
+        <v>349</v>
+      </c>
+      <c r="B123" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>362</v>
+        <v>351</v>
+      </c>
+      <c r="B124" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>371</v>
+        <v>365</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed missing keys in language for Spanish
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFAB6D3-45A0-4482-93D6-C66C72510B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C53A0B-55DB-4721-AA48-41598657E191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5700" yWindow="3795" windowWidth="22875" windowHeight="15420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5700" yWindow="3795" windowWidth="22875" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="393">
   <si>
     <t>Key</t>
   </si>
@@ -1548,8 +1548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D138"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="A138" sqref="A138"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2750,10 +2750,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A083F05-0FAA-4E78-9E79-0348AF6ADFB8}">
-  <dimension ref="A1:D134"/>
+  <dimension ref="A1:D138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="A132" sqref="A132"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3852,16 +3852,36 @@
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>387</v>
+        <v>371</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>388</v>
+        <v>372</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
         <v>389</v>
       </c>
     </row>

</xml_diff>